<commit_message>
Add pas_021, 027, 029 CSV FIles
</commit_message>
<xml_diff>
--- a/src/pgsql/adif-pas/adif-pas-master.xlsx
+++ b/src/pgsql/adif-pas/adif-pas-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Git\Projects\ards-tools\src\pgsql\adif-pas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D8D12E-EA55-477D-8283-9C7D7C10BC0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4127BD6-D0BE-4743-89E8-4A26BB87C789}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="828" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="828" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENU-LIST" sheetId="37" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="pas_005" sheetId="47" r:id="rId5"/>
     <sheet name="pas_006" sheetId="48" r:id="rId6"/>
     <sheet name="pas_015" sheetId="49" r:id="rId7"/>
+    <sheet name="pas-021" sheetId="50" r:id="rId8"/>
+    <sheet name="pas_027" sheetId="51" r:id="rId9"/>
+    <sheet name="pas_029" sheetId="52" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -310,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="620">
   <si>
     <t>t</t>
   </si>
@@ -2095,6 +2098,81 @@
   </si>
   <si>
     <t>pas_015_utizone</t>
+  </si>
+  <si>
+    <t>IB</t>
+  </si>
+  <si>
+    <t>Baleares</t>
+  </si>
+  <si>
+    <t>Beleric Is.</t>
+  </si>
+  <si>
+    <t>pas_021</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>Minsk (Minskaya voblasts')</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>Brest (Brestskaya voblasts')</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Grodno (Hrodzenskaya voblasts')</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>Vitebsk (Vitsyebskaya voblasts')</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Mogilev (Mahilyowskaya voblasts')</t>
+  </si>
+  <si>
+    <t>HO</t>
+  </si>
+  <si>
+    <t>Gomel (Homyel'skaya voblasts')</t>
+  </si>
+  <si>
+    <t>Horad Minsk</t>
+  </si>
+  <si>
+    <t>pas_027</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Canary Is.</t>
+  </si>
+  <si>
+    <t>pas_029</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>Las Palmas</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>Tenerife</t>
   </si>
 </sst>
 </file>
@@ -2102,7 +2180,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -2324,7 +2402,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2436,7 +2514,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2466,6 +2544,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2985,6 +3066,90 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DC69E8-80AB-4EA2-B28F-47DFA34FD30B}">
+  <dimension ref="B1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="24" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>504</v>
+      </c>
+      <c r="F1" s="54" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>29</v>
+      </c>
+      <c r="D2" s="68" t="s">
+        <v>616</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>617</v>
+      </c>
+      <c r="F2" s="53" t="str">
+        <f t="shared" ref="F2:F3" si="0">B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|29|GC|Las Palmas</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>29</v>
+      </c>
+      <c r="D3" s="68" t="s">
+        <v>618</v>
+      </c>
+      <c r="E3" s="68" t="s">
+        <v>619</v>
+      </c>
+      <c r="F3" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>2|29|TF|Tenerife</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="37" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="37" t="s">
+        <v>614</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E404"/>
@@ -13262,15 +13427,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B18DCC7-E659-4BBC-994E-EFC06234585C}">
   <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13683,8 +13848,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13750,7 +13917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E94F41-E17E-4B9C-9C63-31535A794C71}">
   <dimension ref="B1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13907,7 +14074,7 @@
         <v>2</v>
       </c>
       <c r="L3" s="8">
-        <f t="shared" ref="L3:L42" si="3">B3</f>
+        <f t="shared" ref="L3:L16" si="3">B3</f>
         <v>2</v>
       </c>
       <c r="M3" s="8">
@@ -14641,7 +14808,7 @@
         <v>16</v>
       </c>
       <c r="L17" s="23">
-        <f>B16</f>
+        <f t="shared" ref="L17:L40" si="5">B16</f>
         <v>15</v>
       </c>
       <c r="M17" s="23">
@@ -14693,7 +14860,7 @@
         <v>17</v>
       </c>
       <c r="L18" s="8">
-        <f>B17</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="M18" s="8">
@@ -14745,7 +14912,7 @@
         <v>18</v>
       </c>
       <c r="L19" s="8">
-        <f>B18</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="M19" s="8">
@@ -14797,7 +14964,7 @@
         <v>19</v>
       </c>
       <c r="L20" s="8">
-        <f>B19</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="M20" s="8">
@@ -14849,7 +15016,7 @@
         <v>20</v>
       </c>
       <c r="L21" s="8">
-        <f>B20</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="M21" s="8">
@@ -14901,7 +15068,7 @@
         <v>21</v>
       </c>
       <c r="L22" s="8">
-        <f>B21</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="M22" s="8">
@@ -14955,7 +15122,7 @@
         <v>22</v>
       </c>
       <c r="L23" s="8">
-        <f>B22</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="M23" s="8">
@@ -15007,7 +15174,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="8">
-        <f>B23</f>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="M24" s="8">
@@ -15059,7 +15226,7 @@
         <v>24</v>
       </c>
       <c r="L25" s="8">
-        <f>B24</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="M25" s="8">
@@ -15111,7 +15278,7 @@
         <v>25</v>
       </c>
       <c r="L26" s="8">
-        <f>B25</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="M26" s="8">
@@ -15165,7 +15332,7 @@
         <v>26</v>
       </c>
       <c r="L27" s="8">
-        <f>B26</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="M27" s="8">
@@ -15217,7 +15384,7 @@
         <v>27</v>
       </c>
       <c r="L28" s="8">
-        <f>B27</f>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="M28" s="8">
@@ -15269,7 +15436,7 @@
         <v>28</v>
       </c>
       <c r="L29" s="8">
-        <f>B28</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="M29" s="8">
@@ -15321,7 +15488,7 @@
         <v>29</v>
       </c>
       <c r="L30" s="8">
-        <f>B29</f>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="M30" s="8">
@@ -15373,7 +15540,7 @@
         <v>30</v>
       </c>
       <c r="L31" s="8">
-        <f>B30</f>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="M31" s="8">
@@ -15425,7 +15592,7 @@
         <v>31</v>
       </c>
       <c r="L32" s="8">
-        <f>B31</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="M32" s="8">
@@ -15477,7 +15644,7 @@
         <v>32</v>
       </c>
       <c r="L33" s="8">
-        <f>B32</f>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="M33" s="8">
@@ -15529,7 +15696,7 @@
         <v>33</v>
       </c>
       <c r="L34" s="8">
-        <f>B33</f>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="M34" s="8">
@@ -15585,7 +15752,7 @@
         <v>34</v>
       </c>
       <c r="L35" s="8">
-        <f>B34</f>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="M35" s="8">
@@ -15637,7 +15804,7 @@
         <v>35</v>
       </c>
       <c r="L36" s="8">
-        <f>B35</f>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="M36" s="8">
@@ -15691,7 +15858,7 @@
         <v>36</v>
       </c>
       <c r="L37" s="8">
-        <f>B36</f>
+        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="M37" s="8">
@@ -15743,7 +15910,7 @@
         <v>37</v>
       </c>
       <c r="L38" s="8">
-        <f>B37</f>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="M38" s="8">
@@ -15795,7 +15962,7 @@
         <v>38</v>
       </c>
       <c r="L39" s="8">
-        <f>B38</f>
+        <f t="shared" si="5"/>
         <v>37</v>
       </c>
       <c r="M39" s="8">
@@ -15834,7 +16001,7 @@
         <v>39</v>
       </c>
       <c r="L40" s="8">
-        <f>B39</f>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="M40" s="8">
@@ -15892,4 +16059,245 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DAA529-7071-4254-87B0-DF8867DDA350}">
+  <dimension ref="B1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="24" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>504</v>
+      </c>
+      <c r="F1" s="54" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>21</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>595</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>596</v>
+      </c>
+      <c r="F2" s="53" t="str">
+        <f>B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|21|IB|Baleares</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="37" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="37" t="s">
+        <v>597</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5C29C6-033F-4181-8CBE-3172A9188B6A}">
+  <dimension ref="B1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="24" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>504</v>
+      </c>
+      <c r="F1" s="54" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>599</v>
+      </c>
+      <c r="E2" t="s">
+        <v>600</v>
+      </c>
+      <c r="F2" s="53" t="str">
+        <f t="shared" ref="F2:F8" si="0">B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|27|MI|Minsk (Minskaya voblasts')</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>601</v>
+      </c>
+      <c r="E3" t="s">
+        <v>602</v>
+      </c>
+      <c r="F3" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>2|27|BR|Brest (Brestskaya voblasts')</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>603</v>
+      </c>
+      <c r="E4" t="s">
+        <v>604</v>
+      </c>
+      <c r="F4" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>3|27|HR|Grodno (Hrodzenskaya voblasts')</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" s="8">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>605</v>
+      </c>
+      <c r="E5" t="s">
+        <v>606</v>
+      </c>
+      <c r="F5" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>4|27|VI|Vitebsk (Vitsyebskaya voblasts')</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>607</v>
+      </c>
+      <c r="E6" t="s">
+        <v>608</v>
+      </c>
+      <c r="F6" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>5|27|MA|Mogilev (Mahilyowskaya voblasts')</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="8">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>609</v>
+      </c>
+      <c r="E7" t="s">
+        <v>610</v>
+      </c>
+      <c r="F7" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>6|27|HO|Gomel (Homyel'skaya voblasts')</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>521</v>
+      </c>
+      <c r="E8" t="s">
+        <v>611</v>
+      </c>
+      <c r="F8" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>7|27|HM|Horad Minsk</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="37" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="37" t="s">
+        <v>613</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add pas_144, 147, 148,148, 150 and 151 CSV Files.
</commit_message>
<xml_diff>
--- a/src/pgsql/adif-pas/adif-pas-master.xlsx
+++ b/src/pgsql/adif-pas/adif-pas-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Git\Projects\ards-tools\src\pgsql\adif-pas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245B6C37-B9B3-46AD-B134-C53B5C5EBE58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604E962A-F6A0-48DD-9C5B-FFABC3CAC5DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,6 +41,12 @@
     <sheet name="pas_132" sheetId="68" r:id="rId26"/>
     <sheet name="pas_137" sheetId="69" r:id="rId27"/>
     <sheet name="pas_138" sheetId="70" r:id="rId28"/>
+    <sheet name="pas_144" sheetId="71" r:id="rId29"/>
+    <sheet name="pas_147" sheetId="72" r:id="rId30"/>
+    <sheet name="pas_148" sheetId="73" r:id="rId31"/>
+    <sheet name="psa_149" sheetId="74" r:id="rId32"/>
+    <sheet name="pas_150" sheetId="75" r:id="rId33"/>
+    <sheet name="pas_151" sheetId="76" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -331,7 +337,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="1213">
   <si>
     <t>t</t>
   </si>
@@ -3694,6 +3700,282 @@
   </si>
   <si>
     <t>pas_137</t>
+  </si>
+  <si>
+    <t>psa_144</t>
+  </si>
+  <si>
+    <t>Uraguay</t>
+  </si>
+  <si>
+    <t>Montevideo</t>
+  </si>
+  <si>
+    <t>Canelones</t>
+  </si>
+  <si>
+    <t>San José</t>
+  </si>
+  <si>
+    <t>Colonia</t>
+  </si>
+  <si>
+    <t>Soriano</t>
+  </si>
+  <si>
+    <t>Rio Negro</t>
+  </si>
+  <si>
+    <t>Paysandu</t>
+  </si>
+  <si>
+    <t>Salto</t>
+  </si>
+  <si>
+    <t>Artigsa</t>
+  </si>
+  <si>
+    <t>FD</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>Flores</t>
+  </si>
+  <si>
+    <t>DU</t>
+  </si>
+  <si>
+    <t>Durazno</t>
+  </si>
+  <si>
+    <t>Tacuarembo</t>
+  </si>
+  <si>
+    <t>RV</t>
+  </si>
+  <si>
+    <t>Rivera</t>
+  </si>
+  <si>
+    <t>Maldonado</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>Lavalleja</t>
+  </si>
+  <si>
+    <t>Rocha</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>Treinta y Tres</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>Cerro Largo</t>
+  </si>
+  <si>
+    <t>Lord Howe Is</t>
+  </si>
+  <si>
+    <t>LH</t>
+  </si>
+  <si>
+    <t>psa_147</t>
+  </si>
+  <si>
+    <t>pas_148</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Anzoátegui</t>
+  </si>
+  <si>
+    <t>Apure</t>
+  </si>
+  <si>
+    <t>Aragua</t>
+  </si>
+  <si>
+    <t>Barinas</t>
+  </si>
+  <si>
+    <t>Bolívar</t>
+  </si>
+  <si>
+    <t>Carabobo</t>
+  </si>
+  <si>
+    <t>Cojedes</t>
+  </si>
+  <si>
+    <t>Delta Amacuro</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>Distrito Capital</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>Falcón</t>
+  </si>
+  <si>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>Guárico</t>
+  </si>
+  <si>
+    <t>Lara</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>Mérida</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>Monagas</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>Nueva Esparta</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>Portuguesa</t>
+  </si>
+  <si>
+    <t>SU</t>
+  </si>
+  <si>
+    <t>Sucre</t>
+  </si>
+  <si>
+    <t>Táchira</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>Trujillo</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>Vargas</t>
+  </si>
+  <si>
+    <t>Yaracuy</t>
+  </si>
+  <si>
+    <t>ZU</t>
+  </si>
+  <si>
+    <t>Zulia</t>
+  </si>
+  <si>
+    <t>Açores</t>
+  </si>
+  <si>
+    <t>psa_149</t>
+  </si>
+  <si>
+    <t>Azores</t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>Australian Capital Territory</t>
+  </si>
+  <si>
+    <t>NSW</t>
+  </si>
+  <si>
+    <t>New South Wales</t>
+  </si>
+  <si>
+    <t>VIC</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>QLD</t>
+  </si>
+  <si>
+    <t>Queensland</t>
+  </si>
+  <si>
+    <t>South Australia</t>
+  </si>
+  <si>
+    <t>WA</t>
+  </si>
+  <si>
+    <t>Western Australia</t>
+  </si>
+  <si>
+    <t>TAS</t>
+  </si>
+  <si>
+    <t>Tasmania</t>
+  </si>
+  <si>
+    <t>Northern Territory</t>
+  </si>
+  <si>
+    <t>pas_150</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Malyj Vysotskij</t>
+  </si>
+  <si>
+    <t>pas_151</t>
+  </si>
+  <si>
+    <t>Leningradskaya Oblast</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>pas_144</t>
+  </si>
+  <si>
+    <t>pas_147</t>
+  </si>
+  <si>
+    <t>pas_149</t>
   </si>
 </sst>
 </file>
@@ -4400,11 +4682,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18460EF-30D2-4D9B-9C36-93BDE7059CF7}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4484,7 +4766,7 @@
         <v>999</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f t="shared" ref="D5:D34" si="0">A5&amp;".csv"</f>
+        <f t="shared" ref="D5:D40" si="0">A5&amp;".csv"</f>
         <v>pas_summary.csv</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -5133,6 +5415,138 @@
         <v>407</v>
       </c>
       <c r="F34" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B35" s="6">
+        <v>144</v>
+      </c>
+      <c r="C35" t="str">
+        <f>dxcc!D141</f>
+        <v>URUGUAY</v>
+      </c>
+      <c r="D35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_144.csv</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B36" s="6">
+        <v>147</v>
+      </c>
+      <c r="C36" t="str">
+        <f>dxcc!D144</f>
+        <v>LORD HOWE I.</v>
+      </c>
+      <c r="D36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_147.csv</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B37" s="6">
+        <v>148</v>
+      </c>
+      <c r="C37" t="str">
+        <f>dxcc!D145</f>
+        <v>VENEZUELA</v>
+      </c>
+      <c r="D37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_148.csv</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B38" s="6">
+        <v>149</v>
+      </c>
+      <c r="C38" t="str">
+        <f>dxcc!D146</f>
+        <v>AZORES</v>
+      </c>
+      <c r="D38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_149.csv</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B39" s="6">
+        <v>150</v>
+      </c>
+      <c r="C39" t="str">
+        <f>dxcc!D147</f>
+        <v>AUSTRALIA</v>
+      </c>
+      <c r="D39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_150.csv</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B40" s="6">
+        <v>151</v>
+      </c>
+      <c r="C40" t="str">
+        <f>dxcc!D148</f>
+        <v>MALYJ VYSOTSKIJ I.</v>
+      </c>
+      <c r="D40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_151.csv</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F40" s="6" t="s">
         <v>407</v>
       </c>
     </row>
@@ -9238,7 +9652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B1:F407"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D127" sqref="D127"/>
     </sheetView>
   </sheetViews>
@@ -18910,6 +19324,396 @@
     <row r="5" spans="2:6">
       <c r="F5" s="27" t="s">
         <v>1111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5435EA7-D4D3-4F6C-86F1-F7F3B1FE49E2}">
+  <dimension ref="B1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="38" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>144</v>
+      </c>
+      <c r="D2" t="s">
+        <v>726</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F2" s="53" t="str">
+        <f>B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|144|MO|Montevideo</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>144</v>
+      </c>
+      <c r="D3" t="s">
+        <v>833</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="F3" s="53" t="str">
+        <f t="shared" ref="F3:F20" si="0">B3&amp;"|"&amp;C3&amp;"|"&amp;D3&amp;"|"&amp;E3</f>
+        <v>2|144|CA|Canelones</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>144</v>
+      </c>
+      <c r="D4" t="s">
+        <v>865</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F4" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>3|144|SJ|San José</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>144</v>
+      </c>
+      <c r="D5" t="s">
+        <v>857</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="F5" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>4|144|CO|Colonia</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>144</v>
+      </c>
+      <c r="D6" t="s">
+        <v>791</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F6" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>5|144|SO|Soriano</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>144</v>
+      </c>
+      <c r="D7" t="s">
+        <v>960</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1128</v>
+      </c>
+      <c r="F7" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>6|144|RN|Rio Negro</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>144</v>
+      </c>
+      <c r="D8" t="s">
+        <v>836</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F8" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>7|144|PA|Paysandu</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>144</v>
+      </c>
+      <c r="D9" t="s">
+        <v>763</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F9" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>8|144|SA|Salto</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>144</v>
+      </c>
+      <c r="D10" t="s">
+        <v>713</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F10" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>9|144|AR|Artigsa</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1132</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F11" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>10|144|FD|Florida</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6">
+        <v>144</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F12" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11|144|FS|Flores</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>144</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F13" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>12|144|DU|Durazno</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="6">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6">
+        <v>144</v>
+      </c>
+      <c r="D14" t="s">
+        <v>773</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F14" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>13|144|TA|Tacuarembo</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="6">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6">
+        <v>144</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F15" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>14|144|RV|Rivera</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="6">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6">
+        <v>144</v>
+      </c>
+      <c r="D16" t="s">
+        <v>584</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F16" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>15|144|MA|Maldonado</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="6">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6">
+        <v>144</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1143</v>
+      </c>
+      <c r="F17" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>16|144|LA|Lavalleja</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="6">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>144</v>
+      </c>
+      <c r="D18" t="s">
+        <v>793</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F18" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>17|144|RO|Rocha</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="6">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6">
+        <v>144</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F19" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>18|144|TT|Treinta y Tres</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="6">
+        <v>19</v>
+      </c>
+      <c r="C20" s="6">
+        <v>144</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F20" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>19|144|CL|Cerro Largo</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="F22" s="27" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="F23" s="27" t="s">
+        <v>1122</v>
       </c>
     </row>
   </sheetData>
@@ -21092,6 +21896,910 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FBD1D9-41E6-4978-B2AA-7161DE7D810C}">
+  <dimension ref="B1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="38" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>147</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1149</v>
+      </c>
+      <c r="F2" s="53" t="str">
+        <f>B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|147|LH|Lord Howe Is</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="F4" s="27" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="F5" s="27" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E07F0F4C-5AB4-4B3B-9AF7-47A24C3F2944}">
+  <dimension ref="B1:F28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="58" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="38" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>148</v>
+      </c>
+      <c r="D2" t="s">
+        <v>538</v>
+      </c>
+      <c r="E2" t="s">
+        <v>953</v>
+      </c>
+      <c r="F2" s="53" t="str">
+        <f>B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|148|AM|Amazonas</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>148</v>
+      </c>
+      <c r="D3" t="s">
+        <v>867</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="F3" s="53" t="str">
+        <f t="shared" ref="F3:F25" si="0">B3&amp;"|"&amp;C3&amp;"|"&amp;D3&amp;"|"&amp;E3</f>
+        <v>2|148|AN|Anzoátegui</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>148</v>
+      </c>
+      <c r="D4" t="s">
+        <v>955</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1155</v>
+      </c>
+      <c r="F4" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>3|148|AP|Apure</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>148</v>
+      </c>
+      <c r="D5" t="s">
+        <v>713</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1156</v>
+      </c>
+      <c r="F5" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>4|148|AR|Aragua</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>148</v>
+      </c>
+      <c r="D6" t="s">
+        <v>518</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1157</v>
+      </c>
+      <c r="F6" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>5|148|BA|Barinas</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>148</v>
+      </c>
+      <c r="D7" t="s">
+        <v>759</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1158</v>
+      </c>
+      <c r="F7" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>6|148|BO|Bolívar</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>148</v>
+      </c>
+      <c r="D8" t="s">
+        <v>833</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1159</v>
+      </c>
+      <c r="F8" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>7|148|CA|Carabobo</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>148</v>
+      </c>
+      <c r="D9" t="s">
+        <v>857</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F9" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>8|148|CO|Cojedes</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>148</v>
+      </c>
+      <c r="D10" t="s">
+        <v>801</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1161</v>
+      </c>
+      <c r="F10" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>9|148|DA|Delta Amacuro</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6">
+        <v>148</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F11" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>10|148|DC|Distrito Capital</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6">
+        <v>148</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1165</v>
+      </c>
+      <c r="F12" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>11|148|FA|Falcón</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>148</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1167</v>
+      </c>
+      <c r="F13" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>12|148|GU|Guárico</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="6">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6">
+        <v>148</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1168</v>
+      </c>
+      <c r="F14" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>13|148|LA|Lara</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="6">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6">
+        <v>148</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1170</v>
+      </c>
+      <c r="F15" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>14|148|ME|Mérida</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="6">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6">
+        <v>148</v>
+      </c>
+      <c r="D16" t="s">
+        <v>576</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1171</v>
+      </c>
+      <c r="F16" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>15|148|MI|Miranda</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="6">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6">
+        <v>148</v>
+      </c>
+      <c r="D17" t="s">
+        <v>726</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1172</v>
+      </c>
+      <c r="F17" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>16|148|MO|Monagas</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="6">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>148</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1173</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1174</v>
+      </c>
+      <c r="F18" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>17|148|NE|Nueva Esparta</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="6">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6">
+        <v>148</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1175</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1176</v>
+      </c>
+      <c r="F19" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>18|148|PO|Portuguesa</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="6">
+        <v>19</v>
+      </c>
+      <c r="C20" s="6">
+        <v>148</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1177</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1178</v>
+      </c>
+      <c r="F20" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>19|148|SU|Sucre</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="6">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6">
+        <v>148</v>
+      </c>
+      <c r="D21" t="s">
+        <v>773</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1179</v>
+      </c>
+      <c r="F21" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>20|148|TA|Táchira</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="6">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6">
+        <v>148</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1181</v>
+      </c>
+      <c r="F22" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>21|148|TR|Trujillo</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="6">
+        <v>22</v>
+      </c>
+      <c r="C23" s="6">
+        <v>148</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1182</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1183</v>
+      </c>
+      <c r="F23" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>22|148|VA|Vargas</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="6">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6">
+        <v>148</v>
+      </c>
+      <c r="D24" t="s">
+        <v>546</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1184</v>
+      </c>
+      <c r="F24" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>23|148|YA|Yaracuy</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="6">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6">
+        <v>148</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1185</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F25" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>24|148|ZU|Zulia</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="F27" s="27" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="F28" s="27" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AA3F61-6D96-4B5F-9E29-C0CDEC3516E0}">
+  <dimension ref="B1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="58" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="38" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
+        <v>966</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1187</v>
+      </c>
+      <c r="F2" s="53" t="str">
+        <f>B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|149|AC|Açores</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="F4" s="27" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="F5" s="27" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59DE1505-C995-40A0-AA43-2159905522A5}">
+  <dimension ref="B1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="58" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="38" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>150</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1191</v>
+      </c>
+      <c r="F2" s="53" t="str">
+        <f>B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|150|ACT|Australian Capital Territory</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>150</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="F3" s="53" t="str">
+        <f t="shared" ref="F3:F9" si="0">B3&amp;"|"&amp;C3&amp;"|"&amp;D3&amp;"|"&amp;E3</f>
+        <v>2|150|NSW|New South Wales</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>150</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1194</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1195</v>
+      </c>
+      <c r="F4" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>3|150|VIC|Victoria</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>150</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F5" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>4|150|QLD|Queensland</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>763</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F6" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>5|150|SA|South Australia</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1199</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1200</v>
+      </c>
+      <c r="F7" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>6|150|WA|Western Australia</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1202</v>
+      </c>
+      <c r="F8" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>7|150|TAS|Tasmania</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>150</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F9" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>8|150|NT|Northern Territory</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="F11" s="27" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="F12" s="27" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55B70E8-290D-4974-8E98-B7FE1D89148E}">
+  <dimension ref="B1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7">
+      <c r="B1" s="58" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="58" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>810</v>
+      </c>
+      <c r="G1" s="38" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1&amp;"|"&amp;F1</f>
+        <v>id|dxcc_id|code|subdivision|import_only</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>151</v>
+      </c>
+      <c r="D2" t="s">
+        <v>709</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="53" t="str">
+        <f t="shared" ref="G2:G3" si="0">B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2&amp;"|"&amp;F2</f>
+        <v>1|151|LO|Leningradskaya Oblast|0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>151</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="53" t="str">
+        <f t="shared" si="0"/>
+        <v>2|151|MV|Malyj Vysotskij|1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="G5" s="27" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="G6" s="27" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6FCF9E-88D0-4190-A2F7-F0642BE1327B}">
   <dimension ref="A1:O25"/>

</xml_diff>

<commit_message>
Add pas_225, 227,230,239, and 245 CSV files.
</commit_message>
<xml_diff>
--- a/src/pgsql/adif-pas/adif-pas-master.xlsx
+++ b/src/pgsql/adif-pas/adif-pas-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Git\Projects\ards-tools\src\pgsql\adif-pas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB930B2-D99A-4E28-8F1C-1019EB26D412}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C325F-1E1A-49AC-A2A6-CB3353CCF4A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="828" firstSheet="32" activeTab="50" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ENUM-LIST" sheetId="37" r:id="rId1"/>
@@ -59,6 +59,11 @@
     <sheet name="pas_214" sheetId="86" r:id="rId44"/>
     <sheet name="pas_221" sheetId="87" r:id="rId45"/>
     <sheet name="pas_224" sheetId="88" r:id="rId46"/>
+    <sheet name="pas_225" sheetId="89" r:id="rId47"/>
+    <sheet name="pas_227_x0009_" sheetId="90" r:id="rId48"/>
+    <sheet name="pas_230" sheetId="91" r:id="rId49"/>
+    <sheet name="pas_239" sheetId="93" r:id="rId50"/>
+    <sheet name="psa_245" sheetId="94" r:id="rId51"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -349,7 +354,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3118" uniqueCount="2115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3449" uniqueCount="2355">
   <si>
     <t>t</t>
   </si>
@@ -6694,6 +6699,726 @@
   </si>
   <si>
     <t>pas_224_subdivision</t>
+  </si>
+  <si>
+    <t>pas_225_region.csv</t>
+  </si>
+  <si>
+    <t>Sardinia</t>
+  </si>
+  <si>
+    <t>pas_225_subdivision.csv</t>
+  </si>
+  <si>
+    <t>Sardinia (Sardegna)</t>
+  </si>
+  <si>
+    <t>Cagliari</t>
+  </si>
+  <si>
+    <t>Carbonia-Iglesias</t>
+  </si>
+  <si>
+    <t>Nuoro</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>Ogliastra</t>
+  </si>
+  <si>
+    <t>Oristano</t>
+  </si>
+  <si>
+    <t>OT</t>
+  </si>
+  <si>
+    <t>Olbia-Tempio</t>
+  </si>
+  <si>
+    <t>Sassari</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>MedioCampidano</t>
+  </si>
+  <si>
+    <t>Medio Campidano</t>
+  </si>
+  <si>
+    <t>CREATE TABLE adif.pas_225_subdivision</t>
+  </si>
+  <si>
+    <t>pas_225_region_id INT NOT NULL,</t>
+  </si>
+  <si>
+    <t>code CHAR(2) NOT NULL, -- two char CA, CI, MD, ...</t>
+  </si>
+  <si>
+    <t>import_only BOOLEAN NOT NULL DEFAULT '0',</t>
+  </si>
+  <si>
+    <t>CONSTRAINT pas_225_subdivision_uq UNIQUE (code,subdivision)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE adif.pas_225_region</t>
+  </si>
+  <si>
+    <t>CONSTRAINT pas_225_region_uq UNIQUE (region)</t>
+  </si>
+  <si>
+    <t>pas_225_region</t>
+  </si>
+  <si>
+    <t>pas_225_subdivision</t>
+  </si>
+  <si>
+    <t>pas_227</t>
+  </si>
+  <si>
+    <t>pas_227.csv</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Ain</t>
+  </si>
+  <si>
+    <t>Aisne</t>
+  </si>
+  <si>
+    <t>Allier</t>
+  </si>
+  <si>
+    <t>Alpes-de-Haute-Provence</t>
+  </si>
+  <si>
+    <t>Hautes-Alpes</t>
+  </si>
+  <si>
+    <t>Alpes-Maritimes</t>
+  </si>
+  <si>
+    <t>Ardèche</t>
+  </si>
+  <si>
+    <t>Ardennes</t>
+  </si>
+  <si>
+    <t>Ariège</t>
+  </si>
+  <si>
+    <t>Aube</t>
+  </si>
+  <si>
+    <t>Aude</t>
+  </si>
+  <si>
+    <t>Aveyron</t>
+  </si>
+  <si>
+    <t>Bouches-du-Rhone</t>
+  </si>
+  <si>
+    <t>Calvados</t>
+  </si>
+  <si>
+    <t>Cantal</t>
+  </si>
+  <si>
+    <t>Charente</t>
+  </si>
+  <si>
+    <t>Charente-Maritime</t>
+  </si>
+  <si>
+    <t>Cher</t>
+  </si>
+  <si>
+    <t>Corrèze</t>
+  </si>
+  <si>
+    <t>Cote-d'Or</t>
+  </si>
+  <si>
+    <t>Cotes-d'Armor</t>
+  </si>
+  <si>
+    <t>Creuse</t>
+  </si>
+  <si>
+    <t>Dordogne</t>
+  </si>
+  <si>
+    <t>Doubs</t>
+  </si>
+  <si>
+    <t>Drôme</t>
+  </si>
+  <si>
+    <t>Eure</t>
+  </si>
+  <si>
+    <t>Eure-et-Loir</t>
+  </si>
+  <si>
+    <t>Finistère</t>
+  </si>
+  <si>
+    <t>Gard</t>
+  </si>
+  <si>
+    <t>Haute-Garonne</t>
+  </si>
+  <si>
+    <t>Gere</t>
+  </si>
+  <si>
+    <t>Gironde</t>
+  </si>
+  <si>
+    <t>Hérault</t>
+  </si>
+  <si>
+    <t>Ille-et-Vilaine</t>
+  </si>
+  <si>
+    <t>Indre</t>
+  </si>
+  <si>
+    <t>Indre-et-Loire</t>
+  </si>
+  <si>
+    <t>Isère</t>
+  </si>
+  <si>
+    <t>Jura</t>
+  </si>
+  <si>
+    <t>Landes</t>
+  </si>
+  <si>
+    <t>Loir-et-Cher</t>
+  </si>
+  <si>
+    <t>Loire</t>
+  </si>
+  <si>
+    <t>Haute-Loire</t>
+  </si>
+  <si>
+    <t>Loire-Atlantique</t>
+  </si>
+  <si>
+    <t>Loiret</t>
+  </si>
+  <si>
+    <t>Lot</t>
+  </si>
+  <si>
+    <t>Lot-et-Garonne</t>
+  </si>
+  <si>
+    <t>Lozère</t>
+  </si>
+  <si>
+    <t>Maine-et-Loire</t>
+  </si>
+  <si>
+    <t>Manche</t>
+  </si>
+  <si>
+    <t>Marne</t>
+  </si>
+  <si>
+    <t>Haute-Marne</t>
+  </si>
+  <si>
+    <t>Mayenne</t>
+  </si>
+  <si>
+    <t>Meurthe-et-Moselle</t>
+  </si>
+  <si>
+    <t>Meuse</t>
+  </si>
+  <si>
+    <t>Morbihan</t>
+  </si>
+  <si>
+    <t>Moselle</t>
+  </si>
+  <si>
+    <t>Niëvre</t>
+  </si>
+  <si>
+    <t>Nord</t>
+  </si>
+  <si>
+    <t>Oise</t>
+  </si>
+  <si>
+    <t>Orne</t>
+  </si>
+  <si>
+    <t>Pas-de-Calais</t>
+  </si>
+  <si>
+    <t>Puy-de-Dôme</t>
+  </si>
+  <si>
+    <t>Pyrénées-Atlantiques</t>
+  </si>
+  <si>
+    <t>Hautea-Pyrénées</t>
+  </si>
+  <si>
+    <t>Pyrénées-Orientales</t>
+  </si>
+  <si>
+    <t>Bas-Rhin</t>
+  </si>
+  <si>
+    <t>Haut-Rhin</t>
+  </si>
+  <si>
+    <t>Rhône</t>
+  </si>
+  <si>
+    <t>Haute-Saône</t>
+  </si>
+  <si>
+    <t>Saône-et-Loire</t>
+  </si>
+  <si>
+    <t>Sarthe</t>
+  </si>
+  <si>
+    <t>Savoie</t>
+  </si>
+  <si>
+    <t>Haute-Savoie</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Seine-Maritime</t>
+  </si>
+  <si>
+    <t>Seine-et-Marne</t>
+  </si>
+  <si>
+    <t>Yvelines</t>
+  </si>
+  <si>
+    <t>Deux-Sèvres</t>
+  </si>
+  <si>
+    <t>Somme</t>
+  </si>
+  <si>
+    <t>Tarn</t>
+  </si>
+  <si>
+    <t>Tarn-et-Garonne</t>
+  </si>
+  <si>
+    <t>Var</t>
+  </si>
+  <si>
+    <t>Vaucluse</t>
+  </si>
+  <si>
+    <t>Vendée</t>
+  </si>
+  <si>
+    <t>Vienne</t>
+  </si>
+  <si>
+    <t>Haute-Vienne</t>
+  </si>
+  <si>
+    <t>Vosges</t>
+  </si>
+  <si>
+    <t>Yonne</t>
+  </si>
+  <si>
+    <t>Territoire de Belfort</t>
+  </si>
+  <si>
+    <t>Essonne</t>
+  </si>
+  <si>
+    <t>Hauts-de-Selne</t>
+  </si>
+  <si>
+    <t>Seine-Saint-Denis</t>
+  </si>
+  <si>
+    <t>Val-de-Marne</t>
+  </si>
+  <si>
+    <t>Val-d'Oise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number 20 is missing from the ADIF list on France. </t>
+  </si>
+  <si>
+    <t>pas_230.csv</t>
+  </si>
+  <si>
+    <t>Fed. Rep. Of Germany</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Freistaat Bayern</t>
+  </si>
+  <si>
+    <t>Freie Hansestadt Bremen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>HH</t>
+  </si>
+  <si>
+    <t>Freie und Hansestadt Hamburg</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>RP</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>SH</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Freistaat Sachsen</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>Freistaat Thüringen</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>pas_239.csv</t>
+  </si>
+  <si>
+    <t>GY</t>
+  </si>
+  <si>
+    <t>Gyõr (Gyõr-Moson-Sopron)</t>
+  </si>
+  <si>
+    <t>Vas</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>Zala</t>
+  </si>
+  <si>
+    <t>Komárom (Komárom-Esztergom)</t>
+  </si>
+  <si>
+    <t>VE</t>
+  </si>
+  <si>
+    <t>Veszprém</t>
+  </si>
+  <si>
+    <t>Baranya</t>
+  </si>
+  <si>
+    <t>Somogy</t>
+  </si>
+  <si>
+    <t>Tolna</t>
+  </si>
+  <si>
+    <t>Fejér</t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>Budapest</t>
+  </si>
+  <si>
+    <t>Heves</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>Nógrád</t>
+  </si>
+  <si>
+    <t>Pest</t>
+  </si>
+  <si>
+    <t>Szolnok (Jász-Nagykun-Szolnok)</t>
+  </si>
+  <si>
+    <t>Békés</t>
+  </si>
+  <si>
+    <t>Bács-Kiskun</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Csongrád</t>
+  </si>
+  <si>
+    <t>Borsod (Borsod-Abaúj-Zemplén)</t>
+  </si>
+  <si>
+    <t>Hajdú-Bihar</t>
+  </si>
+  <si>
+    <t>Szabolcs (Szabolcs-Szatmár-Bereg)</t>
+  </si>
+  <si>
+    <t>pas_245.csv</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>CW</t>
+  </si>
+  <si>
+    <t>Carlow (Ceatharlach)</t>
+  </si>
+  <si>
+    <t>Cavan (An Cabhán)</t>
+  </si>
+  <si>
+    <t>Clare (An Clár)</t>
+  </si>
+  <si>
+    <t>Cork (Corcaigh)</t>
+  </si>
+  <si>
+    <t>Donegal (Dún na nGall)</t>
+  </si>
+  <si>
+    <t>Dublin (Baile Áth Cliath)</t>
+  </si>
+  <si>
+    <t>Galway (Gaillimh)</t>
+  </si>
+  <si>
+    <t>Kerry (Ciarraí)</t>
+  </si>
+  <si>
+    <t>Kildare (Cill Dara)</t>
+  </si>
+  <si>
+    <t>Kilkenny (Cill Chainnigh)</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>Laois (Laois)</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t>Leitrim (Liatroim)</t>
+  </si>
+  <si>
+    <t>LK</t>
+  </si>
+  <si>
+    <t>Limerick (Luimneach)</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>Longford (An Longfort)</t>
+  </si>
+  <si>
+    <t>Louth (Lú)</t>
+  </si>
+  <si>
+    <t>Mayo (Maigh Eo)</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>Meath (An Mhí)</t>
+  </si>
+  <si>
+    <t>Monaghan (Muineachán)</t>
+  </si>
+  <si>
+    <t>OY</t>
+  </si>
+  <si>
+    <t>Offaly (Uíbh Fhailí)</t>
+  </si>
+  <si>
+    <t>Roscommon (Ros Comáin)</t>
+  </si>
+  <si>
+    <t>Sligo (Sligeach)</t>
+  </si>
+  <si>
+    <t>Tipperary (Tiobraid Árann)</t>
+  </si>
+  <si>
+    <t>WD</t>
+  </si>
+  <si>
+    <t>Waterford (Port Láirge)</t>
+  </si>
+  <si>
+    <t>WH</t>
+  </si>
+  <si>
+    <t>Westmeath (An Iarmhí)</t>
+  </si>
+  <si>
+    <t>WX</t>
+  </si>
+  <si>
+    <t>Wexford (Loch Garman)</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>Wicklow (Cill Mhantáin)</t>
+  </si>
+  <si>
+    <t>pas_230</t>
+  </si>
+  <si>
+    <t>pas_239</t>
+  </si>
+  <si>
+    <t>pas_245</t>
+  </si>
+  <si>
+    <t>pas_209</t>
+  </si>
+  <si>
+    <t>pas_248</t>
+  </si>
+  <si>
+    <t>pas_256</t>
+  </si>
+  <si>
+    <t>pas_263</t>
+  </si>
+  <si>
+    <t>pas_269</t>
+  </si>
+  <si>
+    <t>pas_272</t>
+  </si>
+  <si>
+    <t>pas_275</t>
+  </si>
+  <si>
+    <t>pas_281</t>
+  </si>
+  <si>
+    <t>pas_284</t>
+  </si>
+  <si>
+    <t>pas_287</t>
+  </si>
+  <si>
+    <t>pas_288</t>
+  </si>
+  <si>
+    <t>pas_291</t>
+  </si>
+  <si>
+    <t>pas_318</t>
+  </si>
+  <si>
+    <t>pas_327</t>
+  </si>
+  <si>
+    <t>pas_339</t>
+  </si>
+  <si>
+    <t>pas_375</t>
+  </si>
+  <si>
+    <t>pas_386</t>
+  </si>
+  <si>
+    <t>pas_387</t>
+  </si>
+  <si>
+    <t>pas_497</t>
+  </si>
+  <si>
+    <t>pas_503</t>
+  </si>
+  <si>
+    <t>pas_504</t>
   </si>
 </sst>
 </file>
@@ -6703,7 +7428,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6821,8 +7546,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6872,6 +7604,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -6953,7 +7690,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6961,8 +7698,9 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -7145,11 +7883,19 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="7" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="Calculation" xfId="6" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="7" builtinId="20"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_pas_052" xfId="5" xr:uid="{AAD3A17B-11FB-4A1D-9A7D-F432A6F984A1}"/>
@@ -7470,18 +8216,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18460EF-30D2-4D9B-9C36-93BDE7059CF7}">
-  <dimension ref="A1:G54"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -7554,7 +8300,7 @@
         <v>999</v>
       </c>
       <c r="D5" s="1" t="str">
-        <f t="shared" ref="D5:D54" si="0">A5&amp;".csv"</f>
+        <f t="shared" ref="D5:D81" si="0">A5&amp;".csv"</f>
         <v>pas_summary.csv</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -8514,20 +9260,20 @@
         <v>407</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
-      <c r="A49" t="s">
-        <v>1637</v>
-      </c>
-      <c r="B49" s="6">
-        <v>212</v>
-      </c>
-      <c r="C49" t="str">
-        <f>dxcc!D208</f>
-        <v>BULGARIA</v>
-      </c>
-      <c r="D49" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>pas_212_region.csv</v>
+    <row r="49" spans="1:7">
+      <c r="A49" s="78" t="s">
+        <v>2334</v>
+      </c>
+      <c r="B49" s="79">
+        <v>209</v>
+      </c>
+      <c r="C49" s="78" t="str">
+        <f>dxcc!D205</f>
+        <v>BELGIUM</v>
+      </c>
+      <c r="D49" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_209.csv</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>407</v>
@@ -8536,9 +9282,9 @@
         <v>407</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B50" s="6">
         <v>212</v>
@@ -8549,7 +9295,7 @@
       </c>
       <c r="D50" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>pas_212_subdivision.csv</v>
+        <v>pas_212_region.csv</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>407</v>
@@ -8558,64 +9304,64 @@
         <v>407</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B51" s="6">
+        <v>212</v>
+      </c>
+      <c r="C51" t="str">
+        <f>dxcc!D208</f>
+        <v>BULGARIA</v>
+      </c>
+      <c r="D51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_212_subdivision.csv</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
         <v>1645</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B52" s="6">
         <v>214</v>
       </c>
-      <c r="C51" t="str">
+      <c r="C52" t="str">
         <f>dxcc!D210</f>
         <v>CORSICA</v>
       </c>
-      <c r="D51" s="1" t="str">
+      <c r="D52" s="1" t="str">
         <f t="shared" si="0"/>
         <v>pas_214.csv</v>
       </c>
-      <c r="E51" s="6" t="s">
+      <c r="E52" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="F51" s="6" t="s">
+      <c r="F52" s="6" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
-      <c r="A52" t="s">
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
         <v>1646</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B53" s="6">
         <v>221</v>
       </c>
-      <c r="C52" t="str">
+      <c r="C53" t="str">
         <f>dxcc!D217</f>
         <v>DENMARK</v>
       </c>
-      <c r="D52" s="1" t="str">
+      <c r="D53" s="1" t="str">
         <f t="shared" si="0"/>
         <v>pas_221.csv</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>407</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" t="s">
-        <v>2113</v>
-      </c>
-      <c r="B53" s="6">
-        <v>224</v>
-      </c>
-      <c r="C53" t="str">
-        <f>dxcc!D220</f>
-        <v>FINLAND</v>
-      </c>
-      <c r="D53" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>pas_224_region.csv</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>407</v>
@@ -8624,9 +9370,9 @@
         <v>407</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="B54" s="6">
         <v>224</v>
@@ -8637,13 +9383,350 @@
       </c>
       <c r="D54" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>pas_224_subdivision.csv</v>
+        <v>pas_224_region.csv</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>407</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>407</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>2114</v>
+      </c>
+      <c r="B55" s="6">
+        <v>224</v>
+      </c>
+      <c r="C55" t="str">
+        <f>dxcc!D220</f>
+        <v>FINLAND</v>
+      </c>
+      <c r="D55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_224_subdivision.csv</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>2138</v>
+      </c>
+      <c r="B56" s="6">
+        <v>225</v>
+      </c>
+      <c r="C56" t="str">
+        <f>dxcc!D221</f>
+        <v>SARDINIA</v>
+      </c>
+      <c r="D56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_225_region.csv</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>2139</v>
+      </c>
+      <c r="B57" s="6">
+        <v>225</v>
+      </c>
+      <c r="C57" t="str">
+        <f>dxcc!D221</f>
+        <v>SARDINIA</v>
+      </c>
+      <c r="D57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_225_subdivision.csv</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>2140</v>
+      </c>
+      <c r="B58" s="6">
+        <v>227</v>
+      </c>
+      <c r="C58" t="str">
+        <f>dxcc!D223</f>
+        <v>FRANCE</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_227.csv</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="G58" t="s">
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>2331</v>
+      </c>
+      <c r="B59" s="6">
+        <v>230</v>
+      </c>
+      <c r="C59" t="str">
+        <f>dxcc!D226</f>
+        <v>FEDERAL REPUBLIC OF GERMANY</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_230.csv</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>2332</v>
+      </c>
+      <c r="B60" s="6">
+        <v>239</v>
+      </c>
+      <c r="C60" t="str">
+        <f>dxcc!D235</f>
+        <v>HUNGARY</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_239.csv</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>2333</v>
+      </c>
+      <c r="B61" s="6">
+        <v>245</v>
+      </c>
+      <c r="C61" t="str">
+        <f>dxcc!D241</f>
+        <v>IRELAND</v>
+      </c>
+      <c r="D61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_245.csv</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>2335</v>
+      </c>
+      <c r="D62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_248.csv</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>2336</v>
+      </c>
+      <c r="D63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_256.csv</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>2337</v>
+      </c>
+      <c r="D64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_263.csv</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>2338</v>
+      </c>
+      <c r="D65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_269.csv</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
+        <v>2339</v>
+      </c>
+      <c r="D66" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_272.csv</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>2340</v>
+      </c>
+      <c r="D67" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_275.csv</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>2341</v>
+      </c>
+      <c r="D68" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_281.csv</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>2342</v>
+      </c>
+      <c r="D69" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_284.csv</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>2343</v>
+      </c>
+      <c r="D70" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_287.csv</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>2344</v>
+      </c>
+      <c r="D71" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_288.csv</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>2345</v>
+      </c>
+      <c r="D72" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_291.csv</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>2346</v>
+      </c>
+      <c r="D73" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_318.csv</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>2347</v>
+      </c>
+      <c r="D74" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_327.csv</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>2348</v>
+      </c>
+      <c r="D75" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_339.csv</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>2349</v>
+      </c>
+      <c r="D76" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_375.csv</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>2350</v>
+      </c>
+      <c r="D77" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_386.csv</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>2351</v>
+      </c>
+      <c r="D78" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_387.csv</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>2352</v>
+      </c>
+      <c r="D79" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_497.csv</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>2353</v>
+      </c>
+      <c r="D80" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_503.csv</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>2354</v>
+      </c>
+      <c r="D81" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>pas_504.csv</v>
       </c>
     </row>
   </sheetData>
@@ -28356,9 +29439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F642EE8-FDBC-44E3-9B21-CB8CBC324855}">
   <dimension ref="B1:N128"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -31645,14 +32726,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B472BB40-42FA-42C6-BCBE-E2F477C511E6}">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="2.7109375" style="6" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="6" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
     <col min="6" max="6" width="47.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -31981,7 +33064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB2E3831-8F36-440A-972F-09925986B74F}">
   <dimension ref="B1:M452"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -40872,6 +41955,2448 @@
     <row r="452" spans="3:4">
       <c r="C452" s="1"/>
       <c r="D452" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D58D2BA-EB07-43C0-9469-EED1353C5586}">
+  <dimension ref="B1:N51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="3" style="6" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" style="6" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="6" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="5.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="63" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14">
+      <c r="B1" s="70" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="70" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>1376</v>
+      </c>
+      <c r="E1" s="37" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1</f>
+        <v>id|dxcc_id|region</v>
+      </c>
+      <c r="G1" s="72" t="s">
+        <v>403</v>
+      </c>
+      <c r="H1" s="72" t="s">
+        <v>1375</v>
+      </c>
+      <c r="I1" s="73" t="s">
+        <v>405</v>
+      </c>
+      <c r="J1" s="73" t="s">
+        <v>486</v>
+      </c>
+      <c r="K1" s="73" t="s">
+        <v>810</v>
+      </c>
+      <c r="L1" s="37" t="str">
+        <f>G1&amp;"|"&amp;H1&amp;"|"&amp;I1&amp;"|"&amp;J1&amp;"|"&amp;K1</f>
+        <v>id|pas_206_region_id|code|subdivision|import_only</v>
+      </c>
+      <c r="N1" s="66" t="s">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>225</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2118</v>
+      </c>
+      <c r="E2" s="52" t="str">
+        <f t="shared" ref="E2" si="0">B2&amp;"|"&amp;C2&amp;"|"&amp;D2</f>
+        <v>1|225|Sardinia (Sardegna)</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>833</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2119</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="52" t="str">
+        <f t="shared" ref="L2:L10" si="1">G2&amp;"|"&amp;H2&amp;"|"&amp;I2&amp;"|"&amp;J2&amp;"|"&amp;K2</f>
+        <v>1|1|CA|Cagliari|0</v>
+      </c>
+      <c r="N2" s="66" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14">
+      <c r="G3" s="6">
+        <v>2</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>856</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2120</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>2|1|CI|Carbonia-Iglesias|0</v>
+      </c>
+      <c r="N3" s="67" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
+      <c r="E4" s="27" t="s">
+        <v>2115</v>
+      </c>
+      <c r="G4" s="6">
+        <v>3</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>777</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2130</v>
+      </c>
+      <c r="K4" s="6">
+        <v>1</v>
+      </c>
+      <c r="L4" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>3|1|MD|Medio Campidano|1</v>
+      </c>
+      <c r="N4" s="67" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14">
+      <c r="E5" s="27" t="s">
+        <v>2116</v>
+      </c>
+      <c r="G5" s="6">
+        <v>4</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2121</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>4|1|NU|Nuoro|0</v>
+      </c>
+      <c r="N5" s="67" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
+      <c r="G6" s="6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2122</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2123</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>5|1|OG|Ogliastra|0</v>
+      </c>
+      <c r="N6" s="67" t="s">
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="G7" s="6">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>728</v>
+      </c>
+      <c r="J7" t="s">
+        <v>2124</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>6|1|OR|Oristano|0</v>
+      </c>
+      <c r="N7" s="66" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="G8" s="6">
+        <v>7</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2125</v>
+      </c>
+      <c r="J8" t="s">
+        <v>2126</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>7|1|OT|Olbia-Tempio|0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="G9" s="6">
+        <v>8</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>838</v>
+      </c>
+      <c r="J9" t="s">
+        <v>2127</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0</v>
+      </c>
+      <c r="L9" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>8|1|SS|Sassari|0</v>
+      </c>
+      <c r="N9" s="66" t="s">
+        <v>2131</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="G10" s="6">
+        <v>9</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>2128</v>
+      </c>
+      <c r="J10" t="s">
+        <v>2129</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0</v>
+      </c>
+      <c r="L10" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>9|1|VS|MedioCampidano|0</v>
+      </c>
+      <c r="N10" s="66" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
+      <c r="N11" s="67" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="L12" s="27" t="s">
+        <v>2117</v>
+      </c>
+      <c r="N12" s="67" t="s">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="L13" s="27" t="s">
+        <v>2116</v>
+      </c>
+      <c r="N13" s="67" t="s">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
+      <c r="N14" s="67" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14">
+      <c r="N15" s="67" t="s">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="N16" s="67" t="s">
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="17" spans="3:14">
+      <c r="N17" s="66" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14">
+      <c r="C19" s="76"/>
+      <c r="E19" s="69"/>
+    </row>
+    <row r="21" spans="3:14">
+      <c r="E21" s="69"/>
+    </row>
+    <row r="23" spans="3:14">
+      <c r="C23" s="76"/>
+    </row>
+    <row r="25" spans="3:14">
+      <c r="C25" s="76"/>
+    </row>
+    <row r="28" spans="3:14">
+      <c r="E28" s="69"/>
+    </row>
+    <row r="29" spans="3:14">
+      <c r="C29" s="76"/>
+    </row>
+    <row r="40" spans="5:5">
+      <c r="E40" s="69"/>
+    </row>
+    <row r="51" spans="5:5">
+      <c r="E51" s="69"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{193BA0F8-5632-41D4-B690-969D54FB1B79}">
+  <dimension ref="B1:F98"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" style="6" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="40" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="37" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>227</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2143</v>
+      </c>
+      <c r="F2" s="52" t="str">
+        <f>B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|227|1|Ain</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>227</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2144</v>
+      </c>
+      <c r="F3" s="52" t="str">
+        <f t="shared" ref="F3:F66" si="0">B3&amp;"|"&amp;C3&amp;"|"&amp;D3&amp;"|"&amp;E3</f>
+        <v>2|227|2|Aisne</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>227</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2145</v>
+      </c>
+      <c r="F4" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>3|227|3|Allier</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>227</v>
+      </c>
+      <c r="D5" s="6">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2146</v>
+      </c>
+      <c r="F5" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>4|227|4|Alpes-de-Haute-Provence</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>227</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2147</v>
+      </c>
+      <c r="F6" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>5|227|5|Hautes-Alpes</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>227</v>
+      </c>
+      <c r="D7" s="6">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2148</v>
+      </c>
+      <c r="F7" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>6|227|6|Alpes-Maritimes</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>227</v>
+      </c>
+      <c r="D8" s="6">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2149</v>
+      </c>
+      <c r="F8" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>7|227|7|Ardèche</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>227</v>
+      </c>
+      <c r="D9" s="6">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2150</v>
+      </c>
+      <c r="F9" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>8|227|8|Ardennes</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>227</v>
+      </c>
+      <c r="D10" s="6">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2151</v>
+      </c>
+      <c r="F10" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>9|227|9|Ariège</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6">
+        <v>227</v>
+      </c>
+      <c r="D11" s="6">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2152</v>
+      </c>
+      <c r="F11" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>10|227|10|Aube</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6">
+        <v>227</v>
+      </c>
+      <c r="D12" s="6">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2153</v>
+      </c>
+      <c r="F12" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>11|227|11|Aude</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>227</v>
+      </c>
+      <c r="D13" s="6">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2154</v>
+      </c>
+      <c r="F13" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>12|227|12|Aveyron</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="6">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6">
+        <v>227</v>
+      </c>
+      <c r="D14" s="6">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2155</v>
+      </c>
+      <c r="F14" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>13|227|13|Bouches-du-Rhone</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="6">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6">
+        <v>227</v>
+      </c>
+      <c r="D15" s="6">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2156</v>
+      </c>
+      <c r="F15" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>14|227|14|Calvados</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="6">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6">
+        <v>227</v>
+      </c>
+      <c r="D16" s="6">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2157</v>
+      </c>
+      <c r="F16" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>15|227|15|Cantal</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="6">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6">
+        <v>227</v>
+      </c>
+      <c r="D17" s="6">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2158</v>
+      </c>
+      <c r="F17" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>16|227|16|Charente</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="6">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>227</v>
+      </c>
+      <c r="D18" s="6">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2159</v>
+      </c>
+      <c r="F18" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>17|227|17|Charente-Maritime</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="6">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6">
+        <v>227</v>
+      </c>
+      <c r="D19" s="6">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2160</v>
+      </c>
+      <c r="F19" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>18|227|18|Cher</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="6">
+        <v>19</v>
+      </c>
+      <c r="C20" s="6">
+        <v>227</v>
+      </c>
+      <c r="D20" s="6">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2161</v>
+      </c>
+      <c r="F20" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>19|227|19|Corrèze</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="6">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6">
+        <v>227</v>
+      </c>
+      <c r="D21" s="6">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2162</v>
+      </c>
+      <c r="F21" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>20|227|21|Cote-d'Or</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="6">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6">
+        <v>227</v>
+      </c>
+      <c r="D22" s="6">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2163</v>
+      </c>
+      <c r="F22" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>21|227|22|Cotes-d'Armor</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="6">
+        <v>22</v>
+      </c>
+      <c r="C23" s="6">
+        <v>227</v>
+      </c>
+      <c r="D23" s="6">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2164</v>
+      </c>
+      <c r="F23" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>22|227|23|Creuse</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="6">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6">
+        <v>227</v>
+      </c>
+      <c r="D24" s="6">
+        <v>24</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2165</v>
+      </c>
+      <c r="F24" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>23|227|24|Dordogne</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="6">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6">
+        <v>227</v>
+      </c>
+      <c r="D25" s="6">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2166</v>
+      </c>
+      <c r="F25" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>24|227|25|Doubs</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="6">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6">
+        <v>227</v>
+      </c>
+      <c r="D26" s="6">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2167</v>
+      </c>
+      <c r="F26" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>25|227|26|Drôme</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="6">
+        <v>26</v>
+      </c>
+      <c r="C27" s="6">
+        <v>227</v>
+      </c>
+      <c r="D27" s="6">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2168</v>
+      </c>
+      <c r="F27" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>26|227|27|Eure</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="6">
+        <v>27</v>
+      </c>
+      <c r="C28" s="6">
+        <v>227</v>
+      </c>
+      <c r="D28" s="6">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2169</v>
+      </c>
+      <c r="F28" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>27|227|28|Eure-et-Loir</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="6">
+        <v>28</v>
+      </c>
+      <c r="C29" s="6">
+        <v>227</v>
+      </c>
+      <c r="D29" s="6">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2170</v>
+      </c>
+      <c r="F29" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>28|227|29|Finistère</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="6">
+        <v>29</v>
+      </c>
+      <c r="C30" s="6">
+        <v>227</v>
+      </c>
+      <c r="D30" s="6">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2171</v>
+      </c>
+      <c r="F30" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>29|227|30|Gard</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="6">
+        <v>30</v>
+      </c>
+      <c r="C31" s="6">
+        <v>227</v>
+      </c>
+      <c r="D31" s="6">
+        <v>31</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F31" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>30|227|31|Haute-Garonne</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="6">
+        <v>31</v>
+      </c>
+      <c r="C32" s="6">
+        <v>227</v>
+      </c>
+      <c r="D32" s="6">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2173</v>
+      </c>
+      <c r="F32" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>31|227|32|Gere</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="6">
+        <v>32</v>
+      </c>
+      <c r="C33" s="6">
+        <v>227</v>
+      </c>
+      <c r="D33" s="6">
+        <v>33</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2174</v>
+      </c>
+      <c r="F33" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>32|227|33|Gironde</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="6">
+        <v>33</v>
+      </c>
+      <c r="C34" s="6">
+        <v>227</v>
+      </c>
+      <c r="D34" s="6">
+        <v>34</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2175</v>
+      </c>
+      <c r="F34" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>33|227|34|Hérault</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="6">
+        <v>34</v>
+      </c>
+      <c r="C35" s="6">
+        <v>227</v>
+      </c>
+      <c r="D35" s="6">
+        <v>35</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2176</v>
+      </c>
+      <c r="F35" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>34|227|35|Ille-et-Vilaine</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="6">
+        <v>35</v>
+      </c>
+      <c r="C36" s="6">
+        <v>227</v>
+      </c>
+      <c r="D36" s="6">
+        <v>36</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2177</v>
+      </c>
+      <c r="F36" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>35|227|36|Indre</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="6">
+        <v>36</v>
+      </c>
+      <c r="C37" s="6">
+        <v>227</v>
+      </c>
+      <c r="D37" s="6">
+        <v>37</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2178</v>
+      </c>
+      <c r="F37" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>36|227|37|Indre-et-Loire</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="6">
+        <v>37</v>
+      </c>
+      <c r="C38" s="6">
+        <v>227</v>
+      </c>
+      <c r="D38" s="6">
+        <v>38</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2179</v>
+      </c>
+      <c r="F38" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>37|227|38|Isère</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="6">
+        <v>38</v>
+      </c>
+      <c r="C39" s="6">
+        <v>227</v>
+      </c>
+      <c r="D39" s="6">
+        <v>39</v>
+      </c>
+      <c r="E39" t="s">
+        <v>2180</v>
+      </c>
+      <c r="F39" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>38|227|39|Jura</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="6">
+        <v>39</v>
+      </c>
+      <c r="C40" s="6">
+        <v>227</v>
+      </c>
+      <c r="D40" s="6">
+        <v>40</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2181</v>
+      </c>
+      <c r="F40" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>39|227|40|Landes</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="6">
+        <v>40</v>
+      </c>
+      <c r="C41" s="6">
+        <v>227</v>
+      </c>
+      <c r="D41" s="6">
+        <v>41</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2182</v>
+      </c>
+      <c r="F41" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>40|227|41|Loir-et-Cher</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="6">
+        <v>41</v>
+      </c>
+      <c r="C42" s="6">
+        <v>227</v>
+      </c>
+      <c r="D42" s="6">
+        <v>42</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2183</v>
+      </c>
+      <c r="F42" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>41|227|42|Loire</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="6">
+        <v>42</v>
+      </c>
+      <c r="C43" s="6">
+        <v>227</v>
+      </c>
+      <c r="D43" s="6">
+        <v>43</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2184</v>
+      </c>
+      <c r="F43" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>42|227|43|Haute-Loire</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="6">
+        <v>43</v>
+      </c>
+      <c r="C44" s="6">
+        <v>227</v>
+      </c>
+      <c r="D44" s="6">
+        <v>44</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2185</v>
+      </c>
+      <c r="F44" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>43|227|44|Loire-Atlantique</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="6">
+        <v>44</v>
+      </c>
+      <c r="C45" s="6">
+        <v>227</v>
+      </c>
+      <c r="D45" s="6">
+        <v>45</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2186</v>
+      </c>
+      <c r="F45" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>44|227|45|Loiret</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="6">
+        <v>45</v>
+      </c>
+      <c r="C46" s="6">
+        <v>227</v>
+      </c>
+      <c r="D46" s="6">
+        <v>46</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2187</v>
+      </c>
+      <c r="F46" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>45|227|46|Lot</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="B47" s="6">
+        <v>46</v>
+      </c>
+      <c r="C47" s="6">
+        <v>227</v>
+      </c>
+      <c r="D47" s="6">
+        <v>47</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2188</v>
+      </c>
+      <c r="F47" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>46|227|47|Lot-et-Garonne</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="6">
+        <v>47</v>
+      </c>
+      <c r="C48" s="6">
+        <v>227</v>
+      </c>
+      <c r="D48" s="6">
+        <v>48</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2189</v>
+      </c>
+      <c r="F48" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>47|227|48|Lozère</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="6">
+        <v>48</v>
+      </c>
+      <c r="C49" s="6">
+        <v>227</v>
+      </c>
+      <c r="D49" s="6">
+        <v>49</v>
+      </c>
+      <c r="E49" t="s">
+        <v>2190</v>
+      </c>
+      <c r="F49" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>48|227|49|Maine-et-Loire</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50" s="6">
+        <v>49</v>
+      </c>
+      <c r="C50" s="6">
+        <v>227</v>
+      </c>
+      <c r="D50" s="6">
+        <v>50</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2191</v>
+      </c>
+      <c r="F50" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>49|227|50|Manche</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51" s="6">
+        <v>50</v>
+      </c>
+      <c r="C51" s="6">
+        <v>227</v>
+      </c>
+      <c r="D51" s="6">
+        <v>51</v>
+      </c>
+      <c r="E51" t="s">
+        <v>2192</v>
+      </c>
+      <c r="F51" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>50|227|51|Marne</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="6">
+        <v>51</v>
+      </c>
+      <c r="C52" s="6">
+        <v>227</v>
+      </c>
+      <c r="D52" s="6">
+        <v>52</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2193</v>
+      </c>
+      <c r="F52" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>51|227|52|Haute-Marne</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="6">
+        <v>52</v>
+      </c>
+      <c r="C53" s="6">
+        <v>227</v>
+      </c>
+      <c r="D53" s="6">
+        <v>53</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2194</v>
+      </c>
+      <c r="F53" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>52|227|53|Mayenne</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="6">
+        <v>53</v>
+      </c>
+      <c r="C54" s="6">
+        <v>227</v>
+      </c>
+      <c r="D54" s="6">
+        <v>54</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2195</v>
+      </c>
+      <c r="F54" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>53|227|54|Meurthe-et-Moselle</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="6">
+        <v>54</v>
+      </c>
+      <c r="C55" s="6">
+        <v>227</v>
+      </c>
+      <c r="D55" s="6">
+        <v>55</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2196</v>
+      </c>
+      <c r="F55" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>54|227|55|Meuse</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56" s="6">
+        <v>55</v>
+      </c>
+      <c r="C56" s="6">
+        <v>227</v>
+      </c>
+      <c r="D56" s="6">
+        <v>56</v>
+      </c>
+      <c r="E56" t="s">
+        <v>2197</v>
+      </c>
+      <c r="F56" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>55|227|56|Morbihan</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="6">
+        <v>56</v>
+      </c>
+      <c r="C57" s="6">
+        <v>227</v>
+      </c>
+      <c r="D57" s="6">
+        <v>57</v>
+      </c>
+      <c r="E57" t="s">
+        <v>2198</v>
+      </c>
+      <c r="F57" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>56|227|57|Moselle</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58" s="6">
+        <v>57</v>
+      </c>
+      <c r="C58" s="6">
+        <v>227</v>
+      </c>
+      <c r="D58" s="6">
+        <v>58</v>
+      </c>
+      <c r="E58" t="s">
+        <v>2199</v>
+      </c>
+      <c r="F58" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>57|227|58|Niëvre</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="B59" s="6">
+        <v>58</v>
+      </c>
+      <c r="C59" s="6">
+        <v>227</v>
+      </c>
+      <c r="D59" s="6">
+        <v>59</v>
+      </c>
+      <c r="E59" t="s">
+        <v>2200</v>
+      </c>
+      <c r="F59" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>58|227|59|Nord</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6">
+      <c r="B60" s="6">
+        <v>59</v>
+      </c>
+      <c r="C60" s="6">
+        <v>227</v>
+      </c>
+      <c r="D60" s="6">
+        <v>60</v>
+      </c>
+      <c r="E60" t="s">
+        <v>2201</v>
+      </c>
+      <c r="F60" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>59|227|60|Oise</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6">
+      <c r="B61" s="6">
+        <v>60</v>
+      </c>
+      <c r="C61" s="6">
+        <v>227</v>
+      </c>
+      <c r="D61" s="6">
+        <v>61</v>
+      </c>
+      <c r="E61" t="s">
+        <v>2202</v>
+      </c>
+      <c r="F61" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>60|227|61|Orne</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6">
+      <c r="B62" s="6">
+        <v>61</v>
+      </c>
+      <c r="C62" s="6">
+        <v>227</v>
+      </c>
+      <c r="D62" s="6">
+        <v>62</v>
+      </c>
+      <c r="E62" t="s">
+        <v>2203</v>
+      </c>
+      <c r="F62" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>61|227|62|Pas-de-Calais</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63" s="6">
+        <v>62</v>
+      </c>
+      <c r="C63" s="6">
+        <v>227</v>
+      </c>
+      <c r="D63" s="6">
+        <v>63</v>
+      </c>
+      <c r="E63" t="s">
+        <v>2204</v>
+      </c>
+      <c r="F63" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>62|227|63|Puy-de-Dôme</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64" s="6">
+        <v>63</v>
+      </c>
+      <c r="C64" s="6">
+        <v>227</v>
+      </c>
+      <c r="D64" s="6">
+        <v>64</v>
+      </c>
+      <c r="E64" t="s">
+        <v>2205</v>
+      </c>
+      <c r="F64" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>63|227|64|Pyrénées-Atlantiques</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="6">
+        <v>64</v>
+      </c>
+      <c r="C65" s="6">
+        <v>227</v>
+      </c>
+      <c r="D65" s="6">
+        <v>65</v>
+      </c>
+      <c r="E65" t="s">
+        <v>2206</v>
+      </c>
+      <c r="F65" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>64|227|65|Hautea-Pyrénées</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66" s="6">
+        <v>65</v>
+      </c>
+      <c r="C66" s="6">
+        <v>227</v>
+      </c>
+      <c r="D66" s="6">
+        <v>66</v>
+      </c>
+      <c r="E66" t="s">
+        <v>2207</v>
+      </c>
+      <c r="F66" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>65|227|66|Pyrénées-Orientales</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67" s="6">
+        <v>66</v>
+      </c>
+      <c r="C67" s="6">
+        <v>227</v>
+      </c>
+      <c r="D67" s="6">
+        <v>67</v>
+      </c>
+      <c r="E67" t="s">
+        <v>2208</v>
+      </c>
+      <c r="F67" s="52" t="str">
+        <f t="shared" ref="F67:F95" si="1">B67&amp;"|"&amp;C67&amp;"|"&amp;D67&amp;"|"&amp;E67</f>
+        <v>66|227|67|Bas-Rhin</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="6">
+        <v>67</v>
+      </c>
+      <c r="C68" s="6">
+        <v>227</v>
+      </c>
+      <c r="D68" s="6">
+        <v>68</v>
+      </c>
+      <c r="E68" t="s">
+        <v>2209</v>
+      </c>
+      <c r="F68" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>67|227|68|Haut-Rhin</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69" s="6">
+        <v>68</v>
+      </c>
+      <c r="C69" s="6">
+        <v>227</v>
+      </c>
+      <c r="D69" s="6">
+        <v>69</v>
+      </c>
+      <c r="E69" t="s">
+        <v>2210</v>
+      </c>
+      <c r="F69" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>68|227|69|Rhône</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" s="6">
+        <v>69</v>
+      </c>
+      <c r="C70" s="6">
+        <v>227</v>
+      </c>
+      <c r="D70" s="6">
+        <v>70</v>
+      </c>
+      <c r="E70" t="s">
+        <v>2211</v>
+      </c>
+      <c r="F70" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>69|227|70|Haute-Saône</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" s="6">
+        <v>70</v>
+      </c>
+      <c r="C71" s="6">
+        <v>227</v>
+      </c>
+      <c r="D71" s="6">
+        <v>71</v>
+      </c>
+      <c r="E71" t="s">
+        <v>2212</v>
+      </c>
+      <c r="F71" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>70|227|71|Saône-et-Loire</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72" s="6">
+        <v>71</v>
+      </c>
+      <c r="C72" s="6">
+        <v>227</v>
+      </c>
+      <c r="D72" s="6">
+        <v>72</v>
+      </c>
+      <c r="E72" t="s">
+        <v>2213</v>
+      </c>
+      <c r="F72" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>71|227|72|Sarthe</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" s="6">
+        <v>72</v>
+      </c>
+      <c r="C73" s="6">
+        <v>227</v>
+      </c>
+      <c r="D73" s="6">
+        <v>73</v>
+      </c>
+      <c r="E73" t="s">
+        <v>2214</v>
+      </c>
+      <c r="F73" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>72|227|73|Savoie</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74" s="6">
+        <v>73</v>
+      </c>
+      <c r="C74" s="6">
+        <v>227</v>
+      </c>
+      <c r="D74" s="6">
+        <v>74</v>
+      </c>
+      <c r="E74" t="s">
+        <v>2215</v>
+      </c>
+      <c r="F74" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>73|227|74|Haute-Savoie</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" s="6">
+        <v>74</v>
+      </c>
+      <c r="C75" s="6">
+        <v>227</v>
+      </c>
+      <c r="D75" s="6">
+        <v>75</v>
+      </c>
+      <c r="E75" t="s">
+        <v>2216</v>
+      </c>
+      <c r="F75" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>74|227|75|Paris</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6">
+      <c r="B76" s="6">
+        <v>75</v>
+      </c>
+      <c r="C76" s="6">
+        <v>227</v>
+      </c>
+      <c r="D76" s="6">
+        <v>76</v>
+      </c>
+      <c r="E76" t="s">
+        <v>2217</v>
+      </c>
+      <c r="F76" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>75|227|76|Seine-Maritime</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="B77" s="6">
+        <v>76</v>
+      </c>
+      <c r="C77" s="6">
+        <v>227</v>
+      </c>
+      <c r="D77" s="6">
+        <v>77</v>
+      </c>
+      <c r="E77" t="s">
+        <v>2218</v>
+      </c>
+      <c r="F77" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>76|227|77|Seine-et-Marne</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="B78" s="6">
+        <v>77</v>
+      </c>
+      <c r="C78" s="6">
+        <v>227</v>
+      </c>
+      <c r="D78" s="6">
+        <v>78</v>
+      </c>
+      <c r="E78" t="s">
+        <v>2219</v>
+      </c>
+      <c r="F78" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>77|227|78|Yvelines</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6">
+      <c r="B79" s="6">
+        <v>78</v>
+      </c>
+      <c r="C79" s="6">
+        <v>227</v>
+      </c>
+      <c r="D79" s="6">
+        <v>79</v>
+      </c>
+      <c r="E79" t="s">
+        <v>2220</v>
+      </c>
+      <c r="F79" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>78|227|79|Deux-Sèvres</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6">
+      <c r="B80" s="6">
+        <v>79</v>
+      </c>
+      <c r="C80" s="6">
+        <v>227</v>
+      </c>
+      <c r="D80" s="6">
+        <v>80</v>
+      </c>
+      <c r="E80" t="s">
+        <v>2221</v>
+      </c>
+      <c r="F80" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>79|227|80|Somme</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="B81" s="6">
+        <v>80</v>
+      </c>
+      <c r="C81" s="6">
+        <v>227</v>
+      </c>
+      <c r="D81" s="6">
+        <v>81</v>
+      </c>
+      <c r="E81" t="s">
+        <v>2222</v>
+      </c>
+      <c r="F81" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>80|227|81|Tarn</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6">
+      <c r="B82" s="6">
+        <v>81</v>
+      </c>
+      <c r="C82" s="6">
+        <v>227</v>
+      </c>
+      <c r="D82" s="6">
+        <v>82</v>
+      </c>
+      <c r="E82" t="s">
+        <v>2223</v>
+      </c>
+      <c r="F82" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>81|227|82|Tarn-et-Garonne</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6">
+      <c r="B83" s="6">
+        <v>82</v>
+      </c>
+      <c r="C83" s="6">
+        <v>227</v>
+      </c>
+      <c r="D83" s="6">
+        <v>83</v>
+      </c>
+      <c r="E83" t="s">
+        <v>2224</v>
+      </c>
+      <c r="F83" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>82|227|83|Var</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6">
+      <c r="B84" s="6">
+        <v>83</v>
+      </c>
+      <c r="C84" s="6">
+        <v>227</v>
+      </c>
+      <c r="D84" s="6">
+        <v>84</v>
+      </c>
+      <c r="E84" t="s">
+        <v>2225</v>
+      </c>
+      <c r="F84" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>83|227|84|Vaucluse</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6">
+      <c r="B85" s="6">
+        <v>84</v>
+      </c>
+      <c r="C85" s="6">
+        <v>227</v>
+      </c>
+      <c r="D85" s="6">
+        <v>85</v>
+      </c>
+      <c r="E85" t="s">
+        <v>2226</v>
+      </c>
+      <c r="F85" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>84|227|85|Vendée</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6">
+      <c r="B86" s="6">
+        <v>85</v>
+      </c>
+      <c r="C86" s="6">
+        <v>227</v>
+      </c>
+      <c r="D86" s="6">
+        <v>86</v>
+      </c>
+      <c r="E86" t="s">
+        <v>2227</v>
+      </c>
+      <c r="F86" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>85|227|86|Vienne</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6">
+      <c r="B87" s="6">
+        <v>86</v>
+      </c>
+      <c r="C87" s="6">
+        <v>227</v>
+      </c>
+      <c r="D87" s="6">
+        <v>87</v>
+      </c>
+      <c r="E87" t="s">
+        <v>2228</v>
+      </c>
+      <c r="F87" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>86|227|87|Haute-Vienne</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6">
+      <c r="B88" s="6">
+        <v>87</v>
+      </c>
+      <c r="C88" s="6">
+        <v>227</v>
+      </c>
+      <c r="D88" s="6">
+        <v>88</v>
+      </c>
+      <c r="E88" t="s">
+        <v>2229</v>
+      </c>
+      <c r="F88" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>87|227|88|Vosges</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6">
+      <c r="B89" s="6">
+        <v>88</v>
+      </c>
+      <c r="C89" s="6">
+        <v>227</v>
+      </c>
+      <c r="D89" s="6">
+        <v>89</v>
+      </c>
+      <c r="E89" t="s">
+        <v>2230</v>
+      </c>
+      <c r="F89" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>88|227|89|Yonne</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6">
+      <c r="B90" s="6">
+        <v>89</v>
+      </c>
+      <c r="C90" s="6">
+        <v>227</v>
+      </c>
+      <c r="D90" s="6">
+        <v>90</v>
+      </c>
+      <c r="E90" t="s">
+        <v>2231</v>
+      </c>
+      <c r="F90" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>89|227|90|Territoire de Belfort</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6">
+      <c r="B91" s="6">
+        <v>90</v>
+      </c>
+      <c r="C91" s="6">
+        <v>227</v>
+      </c>
+      <c r="D91" s="6">
+        <v>91</v>
+      </c>
+      <c r="E91" t="s">
+        <v>2232</v>
+      </c>
+      <c r="F91" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>90|227|91|Essonne</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6">
+      <c r="B92" s="6">
+        <v>91</v>
+      </c>
+      <c r="C92" s="6">
+        <v>227</v>
+      </c>
+      <c r="D92" s="6">
+        <v>92</v>
+      </c>
+      <c r="E92" t="s">
+        <v>2233</v>
+      </c>
+      <c r="F92" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>91|227|92|Hauts-de-Selne</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6">
+      <c r="B93" s="6">
+        <v>92</v>
+      </c>
+      <c r="C93" s="6">
+        <v>227</v>
+      </c>
+      <c r="D93" s="6">
+        <v>93</v>
+      </c>
+      <c r="E93" t="s">
+        <v>2234</v>
+      </c>
+      <c r="F93" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>92|227|93|Seine-Saint-Denis</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6">
+      <c r="B94" s="6">
+        <v>93</v>
+      </c>
+      <c r="C94" s="6">
+        <v>227</v>
+      </c>
+      <c r="D94" s="6">
+        <v>94</v>
+      </c>
+      <c r="E94" t="s">
+        <v>2235</v>
+      </c>
+      <c r="F94" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>93|227|94|Val-de-Marne</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6">
+      <c r="B95" s="6">
+        <v>94</v>
+      </c>
+      <c r="C95" s="6">
+        <v>227</v>
+      </c>
+      <c r="D95" s="6">
+        <v>95</v>
+      </c>
+      <c r="E95" t="s">
+        <v>2236</v>
+      </c>
+      <c r="F95" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v>94|227|95|Val-d'Oise</v>
+      </c>
+    </row>
+    <row r="97" spans="6:6">
+      <c r="F97" s="27" t="s">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="98" spans="6:6">
+      <c r="F98" s="27" t="s">
+        <v>2142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0436A4-17EB-4D45-B4C4-BB2A560B7AFF}">
+  <dimension ref="B1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" style="6" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="40" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="37" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>230</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2240</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2241</v>
+      </c>
+      <c r="F2" s="52" t="str">
+        <f>B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|230|BB|Brandenburg</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>230</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>2242</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2243</v>
+      </c>
+      <c r="F3" s="52" t="str">
+        <f t="shared" ref="F3:F17" si="0">B3&amp;"|"&amp;C3&amp;"|"&amp;D3&amp;"|"&amp;E3</f>
+        <v>2|230|BE|Berlin</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>230</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2244</v>
+      </c>
+      <c r="F4" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>3|230|BW|Baden-Württemberg</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>230</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2245</v>
+      </c>
+      <c r="F5" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>4|230|BY|Freistaat Bayern</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>230</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>1488</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2246</v>
+      </c>
+      <c r="F6" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>5|230|HB|Freie Hansestadt Bremen</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>230</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>1522</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2247</v>
+      </c>
+      <c r="F7" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>6|230|HE|Hessen</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>230</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>2248</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2249</v>
+      </c>
+      <c r="F8" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>7|230|HH|Freie und Hansestadt Hamburg</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>230</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2250</v>
+      </c>
+      <c r="F9" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>8|230|MV|Mecklenburg-Vorpommern</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>230</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>2251</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2252</v>
+      </c>
+      <c r="F10" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>9|230|NI|Niedersachsen</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6">
+        <v>230</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>2253</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2254</v>
+      </c>
+      <c r="F11" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>10|230|NW|Nordrhein-Westfalen</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6">
+        <v>230</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>2255</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2256</v>
+      </c>
+      <c r="F12" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>11|230|RP|Rheinland-Pfalz</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>230</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2257</v>
+      </c>
+      <c r="F13" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>12|230|SL|Saarland</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="6">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6">
+        <v>230</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>2258</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2259</v>
+      </c>
+      <c r="F14" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>13|230|SH|Schleswig-Holstein</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="6">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6">
+        <v>230</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>1353</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2260</v>
+      </c>
+      <c r="F15" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>14|230|SN|Freistaat Sachsen</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="6">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6">
+        <v>230</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>787</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2261</v>
+      </c>
+      <c r="F16" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>15|230|ST|Sachsen-Anhalt</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="6">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6">
+        <v>230</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>2262</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2263</v>
+      </c>
+      <c r="F17" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>16|230|TH|Freistaat Thüringen</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="F19" s="27" t="s">
+        <v>2238</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="F20" s="27" t="s">
+        <v>2239</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41288,6 +44813,930 @@
     <row r="21" spans="2:7">
       <c r="G21" s="55" t="s">
         <v>491</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CFE2BB-6A78-40E1-A1CF-A32E2911E683}">
+  <dimension ref="B1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" style="6" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="32" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="40" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="37" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>239</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2266</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2267</v>
+      </c>
+      <c r="F2" s="52" t="str">
+        <f>B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|239|GY|Gyõr (Gyõr-Moson-Sopron)</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>239</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1180</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2268</v>
+      </c>
+      <c r="F3" s="52" t="str">
+        <f t="shared" ref="F3:F21" si="0">B3&amp;"|"&amp;C3&amp;"|"&amp;D3&amp;"|"&amp;E3</f>
+        <v>2|239|VA|Vas</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>239</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>2269</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2270</v>
+      </c>
+      <c r="F4" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>3|239|ZA|Zala</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>239</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2271</v>
+      </c>
+      <c r="F5" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>4|239|KO|Komárom (Komárom-Esztergom)</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>239</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2272</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2273</v>
+      </c>
+      <c r="F6" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>5|239|VE|Veszprém</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>239</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2274</v>
+      </c>
+      <c r="F7" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>6|239|BA|Baranya</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>239</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>791</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2275</v>
+      </c>
+      <c r="F8" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>7|239|SO|Somogy</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>239</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2276</v>
+      </c>
+      <c r="F9" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>8|239|TO|Tolna</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>239</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>1520</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2277</v>
+      </c>
+      <c r="F10" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>9|239|FE|Fejér</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6">
+        <v>239</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>2278</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2279</v>
+      </c>
+      <c r="F11" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>10|239|BP|Budapest</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6">
+        <v>239</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>1522</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2280</v>
+      </c>
+      <c r="F12" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>11|239|HE|Heves</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>239</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>2281</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2282</v>
+      </c>
+      <c r="F13" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>12|239|NG|Nógrád</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="6">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6">
+        <v>239</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>765</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2283</v>
+      </c>
+      <c r="F14" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>13|239|PE|Pest</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="6">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6">
+        <v>239</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>1517</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2284</v>
+      </c>
+      <c r="F15" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>14|239|SZ|Szolnok (Jász-Nagykun-Szolnok)</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="6">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6">
+        <v>239</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>2242</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2285</v>
+      </c>
+      <c r="F16" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>15|239|BE|Békés</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="6">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6">
+        <v>239</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>1393</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2286</v>
+      </c>
+      <c r="F17" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>16|239|BN|Bács-Kiskun</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="6">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>239</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>2287</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2288</v>
+      </c>
+      <c r="F18" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>17|239|CS|Csongrád</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="6">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6">
+        <v>239</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>759</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2289</v>
+      </c>
+      <c r="F19" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>18|239|BO|Borsod (Borsod-Abaúj-Zemplén)</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="6">
+        <v>19</v>
+      </c>
+      <c r="C20" s="6">
+        <v>239</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>1488</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2290</v>
+      </c>
+      <c r="F20" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>19|239|HB|Hajdú-Bihar</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="6">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6">
+        <v>239</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>763</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2291</v>
+      </c>
+      <c r="F21" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>20|239|SA|Szabolcs (Szabolcs-Szatmár-Bereg)</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="F23" s="27" t="s">
+        <v>2265</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="F24" s="27" t="s">
+        <v>2264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71420057-4E7D-4F04-BA43-300B46C642CD}">
+  <dimension ref="B1:F30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="2.7109375" style="6" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="6" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="32" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="47.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6">
+      <c r="B1" s="40" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>486</v>
+      </c>
+      <c r="F1" s="37" t="str">
+        <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1</f>
+        <v>id|dxcc_id|code|subdivision</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>245</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2294</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2295</v>
+      </c>
+      <c r="F2" s="52" t="str">
+        <f>B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2</f>
+        <v>1|245|CW|Carlow (Ceatharlach)</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>245</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>795</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2296</v>
+      </c>
+      <c r="F3" s="52" t="str">
+        <f t="shared" ref="F3:F27" si="0">B3&amp;"|"&amp;C3&amp;"|"&amp;D3&amp;"|"&amp;E3</f>
+        <v>2|245|CN|Cavan (An Cabhán)</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6">
+        <v>245</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2297</v>
+      </c>
+      <c r="F4" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>3|245|CE|Clare (An Clár)</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>245</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>886</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2298</v>
+      </c>
+      <c r="F5" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>4|245|C|Cork (Corcaigh)</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
+        <v>245</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>1480</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2299</v>
+      </c>
+      <c r="F6" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>5|245|DL|Donegal (Dún na nGall)</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>245</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>914</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2300</v>
+      </c>
+      <c r="F7" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>6|245|D|Dublin (Baile Áth Cliath)</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="6">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6">
+        <v>245</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>908</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2301</v>
+      </c>
+      <c r="F8" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>7|245|G|Galway (Gaillimh)</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="6">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6">
+        <v>245</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2302</v>
+      </c>
+      <c r="F9" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>8|245|KY|Kerry (Ciarraí)</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="6">
+        <v>9</v>
+      </c>
+      <c r="C10" s="6">
+        <v>245</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2303</v>
+      </c>
+      <c r="F10" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>9|245|KE|Kildare (Cill Dara)</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="6">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6">
+        <v>245</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2304</v>
+      </c>
+      <c r="F11" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>10|245|KK|Kilkenny (Cill Chainnigh)</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6">
+        <v>245</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>2305</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2306</v>
+      </c>
+      <c r="F12" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>11|245|LS|Laois (Laois)</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="6">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6">
+        <v>245</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>2307</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2308</v>
+      </c>
+      <c r="F13" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>12|245|LM|Leitrim (Liatroim)</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="6">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6">
+        <v>245</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>2309</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2310</v>
+      </c>
+      <c r="F14" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>13|245|LK|Limerick (Luimneach)</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="6">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6">
+        <v>245</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>2311</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2312</v>
+      </c>
+      <c r="F15" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>14|245|LD|Longford (An Longfort)</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="6">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6">
+        <v>245</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2313</v>
+      </c>
+      <c r="F16" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>15|245|LH|Louth (Lú)</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="6">
+        <v>16</v>
+      </c>
+      <c r="C17" s="6">
+        <v>245</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2314</v>
+      </c>
+      <c r="F17" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>16|245|MO|Mayo (Maigh Eo)</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="6">
+        <v>17</v>
+      </c>
+      <c r="C18" s="6">
+        <v>245</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>2315</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2316</v>
+      </c>
+      <c r="F18" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>17|245|MH|Meath (An Mhí)</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="6">
+        <v>18</v>
+      </c>
+      <c r="C19" s="6">
+        <v>245</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>862</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2317</v>
+      </c>
+      <c r="F19" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>18|245|MN|Monaghan (Muineachán)</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="6">
+        <v>19</v>
+      </c>
+      <c r="C20" s="6">
+        <v>245</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>2318</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2319</v>
+      </c>
+      <c r="F20" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>19|245|OY|Offaly (Uíbh Fhailí)</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="6">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6">
+        <v>245</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>960</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2320</v>
+      </c>
+      <c r="F21" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>20|245|RN|Roscommon (Ros Comáin)</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="6">
+        <v>21</v>
+      </c>
+      <c r="C22" s="6">
+        <v>245</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>791</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2321</v>
+      </c>
+      <c r="F22" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>21|245|SO|Sligo (Sligeach)</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="6">
+        <v>22</v>
+      </c>
+      <c r="C23" s="6">
+        <v>245</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2322</v>
+      </c>
+      <c r="F23" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>22|245|TA|Tipperary (Tiobraid Árann)</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="6">
+        <v>23</v>
+      </c>
+      <c r="C24" s="6">
+        <v>245</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>2323</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2324</v>
+      </c>
+      <c r="F24" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>23|245|WD|Waterford (Port Láirge)</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="6">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6">
+        <v>245</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>2325</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2326</v>
+      </c>
+      <c r="F25" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>24|245|WH|Westmeath (An Iarmhí)</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="6">
+        <v>25</v>
+      </c>
+      <c r="C26" s="6">
+        <v>245</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>2327</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2328</v>
+      </c>
+      <c r="F26" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>25|245|WX|Wexford (Loch Garman)</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="6">
+        <v>26</v>
+      </c>
+      <c r="C27" s="6">
+        <v>245</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>2329</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2330</v>
+      </c>
+      <c r="F27" s="52" t="str">
+        <f t="shared" si="0"/>
+        <v>26|245|WW|Wicklow (Cill Mhantáin)</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="F29" s="27" t="s">
+        <v>2292</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="F30" s="27" t="s">
+        <v>2293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restructured Primary Admin Subdivision Summaries
</commit_message>
<xml_diff>
--- a/src/pgsql/adif-pas/adif-pas-master.xlsx
+++ b/src/pgsql/adif-pas/adif-pas-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Git\Projects\ards-tools\src\pgsql\adif-pas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF62C4D2-0459-4854-8397-667604F855F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854169EE-A5D1-4CE3-8CE3-CC7CAAC4B4D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5860" uniqueCount="3875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5860" uniqueCount="3881">
   <si>
     <t>t</t>
   </si>
@@ -11999,6 +11999,24 @@
   </si>
   <si>
     <t>Quebec</t>
+  </si>
+  <si>
+    <t>sas_summary_id</t>
+  </si>
+  <si>
+    <t>dxcc_code</t>
+  </si>
+  <si>
+    <t>pas_summary_id SERIAL PRIMARY KEY,</t>
+  </si>
+  <si>
+    <t>dxcc_code INT NOT NULL,</t>
+  </si>
+  <si>
+    <t>pas_subdivision_type_id SERIAL PRIMARY KEY,</t>
+  </si>
+  <si>
+    <t>sas_subdivision_type_id SERIAL PRIMARY KEY,</t>
   </si>
 </sst>
 </file>
@@ -12912,7 +12930,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -29537,22 +29555,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="3.42578125" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="6" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="6" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="23" style="6" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="76.140625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="92.140625" style="25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="3" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="20.42578125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="2.7109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="23" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="20.140625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="67.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -29561,10 +29579,10 @@
         <v>3781</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>403</v>
+        <v>3875</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>413</v>
+        <v>3876</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>414</v>
@@ -29580,27 +29598,27 @@
       </c>
       <c r="H1" s="2" t="str">
         <f>B1&amp;"|"&amp;C1&amp;"|"&amp;D1&amp;"|"&amp;E1&amp;"|"&amp;F1&amp;"|"&amp;G1</f>
-        <v>id|dxcc_id|pas_subdivision_type_id|has_oblast|has_sas|sas_subdivision_type_id</v>
+        <v>sas_summary_id|dxcc_code|pas_subdivision_type_id|has_oblast|has_sas|sas_subdivision_type_id</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>403</v>
+        <v>414</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>418</v>
       </c>
       <c r="M1" s="2" t="str">
         <f>K1&amp;"|"&amp;L1</f>
-        <v>id|pas_subdivision_type</v>
+        <v>pas_subdivision_type_id|pas_subdivision_type</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>403</v>
+        <v>417</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>448</v>
       </c>
       <c r="Q1" s="2" t="str">
         <f>O1&amp;"|"&amp;P1</f>
-        <v>id|sas_subdivision_type</v>
+        <v>sas_subdivision_type_id|sas_subdivision_type</v>
       </c>
       <c r="S1" s="117" t="s">
         <v>3857</v>
@@ -29751,7 +29769,7 @@
         <v>3|Cities/Gun</v>
       </c>
       <c r="S4" s="118" t="s">
-        <v>1361</v>
+        <v>3877</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -29794,7 +29812,7 @@
       </c>
       <c r="Q5" s="50"/>
       <c r="S5" s="118" t="s">
-        <v>1368</v>
+        <v>3878</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -30230,7 +30248,7 @@
         <v>15|OKRES</v>
       </c>
       <c r="S16" s="118" t="s">
-        <v>1361</v>
+        <v>3879</v>
       </c>
     </row>
     <row r="17" spans="2:19">
@@ -30546,7 +30564,7 @@
         <v>23|VOBLAST</v>
       </c>
       <c r="S24" s="118" t="s">
-        <v>1361</v>
+        <v>3880</v>
       </c>
     </row>
     <row r="25" spans="2:19">

</xml_diff>

<commit_message>
Fix joins on pas_summary
</commit_message>
<xml_diff>
--- a/src/pgsql/adif-pas/adif-pas-master.xlsx
+++ b/src/pgsql/adif-pas/adif-pas-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Git\Projects\ards-tools\src\pgsql\adif-pas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8957FF6D-E027-4D86-A5CA-67DEBED86C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A27409E-8246-442D-8BBE-46461B459828}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29673,7 +29673,7 @@
       <c r="F2" s="17">
         <v>0</v>
       </c>
-      <c r="H2" s="49" t="str">
+      <c r="H2" s="2" t="str">
         <f t="shared" ref="H2:H65" si="0">B2&amp;"|"&amp;C2&amp;"|"&amp;D2&amp;"|"&amp;E2&amp;"|"&amp;F2&amp;"|"&amp;G2</f>
         <v>1|1|17|0|0|</v>
       </c>
@@ -29721,7 +29721,7 @@
       <c r="F3" s="17">
         <v>0</v>
       </c>
-      <c r="H3" s="49" t="str">
+      <c r="H3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>2|5|10|0|0|</v>
       </c>
@@ -29773,7 +29773,7 @@
         <f>O2</f>
         <v>1</v>
       </c>
-      <c r="H4" s="49" t="str">
+      <c r="H4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>3|6|21|0|1|1</v>
       </c>
@@ -29825,7 +29825,7 @@
         <f>O3</f>
         <v>2</v>
       </c>
-      <c r="H5" s="49" t="str">
+      <c r="H5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>4|15|22|1|1|2</v>
       </c>
@@ -29865,7 +29865,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="18"/>
-      <c r="H6" s="49" t="str">
+      <c r="H6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>5|21|17|0|0|</v>
       </c>
@@ -29907,7 +29907,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="18"/>
-      <c r="H7" s="49" t="str">
+      <c r="H7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>6|27|23|0|0|</v>
       </c>
@@ -29946,7 +29946,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="18"/>
-      <c r="H8" s="49" t="str">
+      <c r="H8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>7|29|17|0|0|</v>
       </c>
@@ -29985,7 +29985,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="18"/>
-      <c r="H9" s="49" t="str">
+      <c r="H9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>8|32|17|0|0|</v>
       </c>
@@ -30024,7 +30024,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="18"/>
-      <c r="H10" s="49" t="str">
+      <c r="H10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>9|50|21|0|0|</v>
       </c>
@@ -30063,7 +30063,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="18"/>
-      <c r="H11" s="49" t="str">
+      <c r="H11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>10|52|12|0|0|</v>
       </c>
@@ -30105,7 +30105,7 @@
         <f>O3</f>
         <v>2</v>
       </c>
-      <c r="H12" s="49" t="str">
+      <c r="H12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>11|54|14|1|1|2</v>
       </c>
@@ -30145,7 +30145,7 @@
         <f>O3</f>
         <v>2</v>
       </c>
-      <c r="H13" s="49" t="str">
+      <c r="H13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>12|61|14|1|1|2</v>
       </c>
@@ -30184,7 +30184,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="18"/>
-      <c r="H14" s="49" t="str">
+      <c r="H14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>13|70|17|0|0|</v>
       </c>
@@ -30223,7 +30223,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="18"/>
-      <c r="H15" s="49" t="str">
+      <c r="H15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>14|74|6|0|0|</v>
       </c>
@@ -30262,7 +30262,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="18"/>
-      <c r="H16" s="49" t="str">
+      <c r="H16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>15|86|6|0|0|</v>
       </c>
@@ -30301,7 +30301,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="18"/>
-      <c r="H17" s="49" t="str">
+      <c r="H17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>16|100|17|0|0|</v>
       </c>
@@ -30340,7 +30340,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="18"/>
-      <c r="H18" s="49" t="str">
+      <c r="H18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>17|104|6|0|0|</v>
       </c>
@@ -30379,7 +30379,7 @@
         <v>0</v>
       </c>
       <c r="G19" s="18"/>
-      <c r="H19" s="49" t="str">
+      <c r="H19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>18|108|21|0|0|</v>
       </c>
@@ -30421,7 +30421,7 @@
         <f>O2</f>
         <v>1</v>
       </c>
-      <c r="H20" s="49" t="str">
+      <c r="H20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>19|110|21|0|1|1</v>
       </c>
@@ -30458,7 +30458,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="18"/>
-      <c r="H21" s="49" t="str">
+      <c r="H21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>20|112|20|0|0|</v>
       </c>
@@ -30500,7 +30500,7 @@
         <f>O3</f>
         <v>2</v>
       </c>
-      <c r="H22" s="49" t="str">
+      <c r="H22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>21|126|14|1|1|2</v>
       </c>
@@ -30539,7 +30539,7 @@
         <v>0</v>
       </c>
       <c r="G23" s="18"/>
-      <c r="H23" s="49" t="str">
+      <c r="H23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>22|130|14|1|0|</v>
       </c>
@@ -30578,7 +30578,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="18"/>
-      <c r="H24" s="49" t="str">
+      <c r="H24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>23|132|6|0|0|</v>
       </c>
@@ -30620,7 +30620,7 @@
         <f>O3</f>
         <v>2</v>
       </c>
-      <c r="H25" s="49" t="str">
+      <c r="H25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>24|137|17|0|1|2</v>
       </c>
@@ -30659,7 +30659,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="18"/>
-      <c r="H26" s="49" t="str">
+      <c r="H26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>25|138|21|0|0|</v>
       </c>
@@ -30698,7 +30698,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="18"/>
-      <c r="H27" s="49" t="str">
+      <c r="H27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>26|144|6|0|0|</v>
       </c>
@@ -30727,7 +30727,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="18"/>
-      <c r="H28" s="49" t="str">
+      <c r="H28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>27|147|21|0|0|</v>
       </c>
@@ -30756,7 +30756,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="18"/>
-      <c r="H29" s="49" t="str">
+      <c r="H29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>28|148|21|0|0|</v>
       </c>
@@ -30782,7 +30782,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="18"/>
-      <c r="H30" s="49" t="str">
+      <c r="H30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>29|149|8|0|0|</v>
       </c>
@@ -30808,7 +30808,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="18"/>
-      <c r="H31" s="49" t="str">
+      <c r="H31" s="2" t="str">
         <f t="shared" si="0"/>
         <v>30|150|21|0|0|</v>
       </c>
@@ -30837,7 +30837,7 @@
         <f>O3</f>
         <v>2</v>
       </c>
-      <c r="H32" s="49" t="str">
+      <c r="H32" s="2" t="str">
         <f t="shared" si="0"/>
         <v>31|151|14|1|1|2</v>
       </c>
@@ -30863,7 +30863,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="18"/>
-      <c r="H33" s="49" t="str">
+      <c r="H33" s="2" t="str">
         <f t="shared" si="0"/>
         <v>32|153|21|0|0|</v>
       </c>
@@ -30889,7 +30889,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="18"/>
-      <c r="H34" s="49" t="str">
+      <c r="H34" s="2" t="str">
         <f t="shared" si="0"/>
         <v>33|163|17|0|0|</v>
       </c>
@@ -30918,8 +30918,8 @@
         <f>O2</f>
         <v>1</v>
       </c>
-      <c r="H35" s="49" t="str">
-        <f t="shared" si="0"/>
+      <c r="H35" s="2" t="str">
+        <f>B35&amp;"|"&amp;C35&amp;"|"&amp;D35&amp;"|"&amp;E35&amp;"|"&amp;F35&amp;"|"&amp;G35</f>
         <v>34|170|20|0|1|1</v>
       </c>
       <c r="I35" s="16" t="s">
@@ -30947,7 +30947,7 @@
         <f>O4</f>
         <v>3</v>
       </c>
-      <c r="H36" s="49" t="str">
+      <c r="H36" s="2" t="str">
         <f t="shared" si="0"/>
         <v>35|177|16|0|1|3</v>
       </c>
@@ -30973,7 +30973,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="18"/>
-      <c r="H37" s="49" t="str">
+      <c r="H37" s="2" t="str">
         <f t="shared" si="0"/>
         <v>36|179|19|0|0|</v>
       </c>
@@ -31002,7 +31002,7 @@
         <f>O4</f>
         <v>3</v>
       </c>
-      <c r="H38" s="49" t="str">
+      <c r="H38" s="2" t="str">
         <f t="shared" si="0"/>
         <v>37|192|16|0|1|3</v>
       </c>
@@ -31028,7 +31028,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="18"/>
-      <c r="H39" s="49" t="str">
+      <c r="H39" s="2" t="str">
         <f t="shared" si="0"/>
         <v>38|206|7|0|0|</v>
       </c>
@@ -31054,7 +31054,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="18"/>
-      <c r="H40" s="49" t="str">
+      <c r="H40" s="2" t="str">
         <f t="shared" si="0"/>
         <v>39|209|17|0|0|</v>
       </c>
@@ -31080,7 +31080,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="18"/>
-      <c r="H41" s="49" t="str">
+      <c r="H41" s="2" t="str">
         <f t="shared" si="0"/>
         <v>40|212|14|0|0|</v>
       </c>
@@ -31106,7 +31106,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="18"/>
-      <c r="H42" s="49" t="str">
+      <c r="H42" s="2" t="str">
         <f t="shared" si="0"/>
         <v>41|214|6|0|0|</v>
       </c>
@@ -31132,7 +31132,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="18"/>
-      <c r="H43" s="49" t="str">
+      <c r="H43" s="2" t="str">
         <f t="shared" si="0"/>
         <v>42|221|1|0|0|</v>
       </c>
@@ -31158,7 +31158,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="18"/>
-      <c r="H44" s="49" t="str">
+      <c r="H44" s="2" t="str">
         <f t="shared" si="0"/>
         <v>43|224|10|0|0|</v>
       </c>
@@ -31184,7 +31184,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="18"/>
-      <c r="H45" s="49" t="str">
+      <c r="H45" s="2" t="str">
         <f t="shared" si="0"/>
         <v>44|225|17|0|0|</v>
       </c>
@@ -31210,7 +31210,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="18"/>
-      <c r="H46" s="49" t="str">
+      <c r="H46" s="2" t="str">
         <f t="shared" si="0"/>
         <v>45|227|6|0|0|</v>
       </c>
@@ -31236,7 +31236,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="18"/>
-      <c r="H47" s="49" t="str">
+      <c r="H47" s="2" t="str">
         <f t="shared" si="0"/>
         <v>46|230|2|0|0|</v>
       </c>
@@ -31262,7 +31262,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="18"/>
-      <c r="H48" s="49" t="str">
+      <c r="H48" s="2" t="str">
         <f t="shared" si="0"/>
         <v>47|239|13|0|0|</v>
       </c>
@@ -31288,7 +31288,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="18"/>
-      <c r="H49" s="49" t="str">
+      <c r="H49" s="2" t="str">
         <f t="shared" si="0"/>
         <v>48|245|5|0|0|</v>
       </c>
@@ -31314,7 +31314,7 @@
         <v>0</v>
       </c>
       <c r="G50" s="18"/>
-      <c r="H50" s="49" t="str">
+      <c r="H50" s="2" t="str">
         <f t="shared" si="0"/>
         <v>49|248|17|0|0|</v>
       </c>
@@ -31340,7 +31340,7 @@
         <v>0</v>
       </c>
       <c r="G51" s="18"/>
-      <c r="H51" s="49" t="str">
+      <c r="H51" s="2" t="str">
         <f t="shared" si="0"/>
         <v>50|256|8|0|0|</v>
       </c>
@@ -31366,7 +31366,7 @@
         <v>0</v>
       </c>
       <c r="G52" s="18"/>
-      <c r="H52" s="49" t="str">
+      <c r="H52" s="2" t="str">
         <f t="shared" si="0"/>
         <v>51|263|17|0|0|</v>
       </c>
@@ -31392,7 +31392,7 @@
         <v>0</v>
       </c>
       <c r="G53" s="18"/>
-      <c r="H53" s="49" t="str">
+      <c r="H53" s="2" t="str">
         <f t="shared" si="0"/>
         <v>52|269|24|0|0|</v>
       </c>
@@ -31418,7 +31418,7 @@
         <v>0</v>
       </c>
       <c r="G54" s="18"/>
-      <c r="H54" s="49" t="str">
+      <c r="H54" s="2" t="str">
         <f t="shared" si="0"/>
         <v>53|272|8|0|0|</v>
       </c>
@@ -31444,7 +31444,7 @@
         <v>0</v>
       </c>
       <c r="G55" s="18"/>
-      <c r="H55" s="49" t="str">
+      <c r="H55" s="2" t="str">
         <f t="shared" si="0"/>
         <v>54|275|9|0|0|</v>
       </c>
@@ -31470,7 +31470,7 @@
         <v>0</v>
       </c>
       <c r="G56" s="18"/>
-      <c r="H56" s="49" t="str">
+      <c r="H56" s="2" t="str">
         <f t="shared" si="0"/>
         <v>55|281|17|0|0|</v>
       </c>
@@ -31496,7 +31496,7 @@
         <v>0</v>
       </c>
       <c r="G57" s="18"/>
-      <c r="H57" s="49" t="str">
+      <c r="H57" s="2" t="str">
         <f t="shared" si="0"/>
         <v>56|284|11|0|0|</v>
       </c>
@@ -31522,8 +31522,8 @@
         <v>0</v>
       </c>
       <c r="G58" s="18"/>
-      <c r="H58" s="49" t="str">
-        <f t="shared" si="0"/>
+      <c r="H58" s="2" t="str">
+        <f>B58&amp;"|"&amp;C58&amp;"|"&amp;D58&amp;"|"&amp;E58&amp;"|"&amp;F58&amp;"|"&amp;G58</f>
         <v>57|287|3|0|0|</v>
       </c>
       <c r="I58" s="16" t="s">
@@ -31551,7 +31551,7 @@
         <f>O3</f>
         <v>2</v>
       </c>
-      <c r="H59" s="49" t="str">
+      <c r="H59" s="2" t="str">
         <f t="shared" si="0"/>
         <v>58|288|14|0|1|2</v>
       </c>
@@ -31580,7 +31580,7 @@
         <f>O3</f>
         <v>2</v>
       </c>
-      <c r="H60" s="49" t="str">
+      <c r="H60" s="2" t="str">
         <f t="shared" si="0"/>
         <v>59|291|21|0|1|2</v>
       </c>
@@ -31606,7 +31606,7 @@
         <v>0</v>
       </c>
       <c r="G61" s="18"/>
-      <c r="H61" s="49" t="str">
+      <c r="H61" s="2" t="str">
         <f t="shared" si="0"/>
         <v>60|318|17|0|0|</v>
       </c>
@@ -31632,7 +31632,7 @@
         <v>0</v>
       </c>
       <c r="G62" s="18"/>
-      <c r="H62" s="49" t="str">
+      <c r="H62" s="2" t="str">
         <f t="shared" si="0"/>
         <v>61|327|18|0|0|</v>
       </c>
@@ -31661,7 +31661,7 @@
         <f>O4</f>
         <v>3</v>
       </c>
-      <c r="H63" s="49" t="str">
+      <c r="H63" s="2" t="str">
         <f t="shared" si="0"/>
         <v>62|339|16|0|1|3</v>
       </c>
@@ -31687,7 +31687,7 @@
         <v>0</v>
       </c>
       <c r="G64" s="18"/>
-      <c r="H64" s="49" t="str">
+      <c r="H64" s="2" t="str">
         <f t="shared" si="0"/>
         <v>63|375|17|0|0|</v>
       </c>
@@ -31713,7 +31713,7 @@
         <v>0</v>
       </c>
       <c r="G65" s="18"/>
-      <c r="H65" s="49" t="str">
+      <c r="H65" s="2" t="str">
         <f t="shared" si="0"/>
         <v>64|386|5|0|0|</v>
       </c>
@@ -31739,7 +31739,7 @@
         <v>0</v>
       </c>
       <c r="G66" s="18"/>
-      <c r="H66" s="49" t="str">
+      <c r="H66" s="2" t="str">
         <f t="shared" ref="H66:H69" si="3">B66&amp;"|"&amp;C66&amp;"|"&amp;D66&amp;"|"&amp;E66&amp;"|"&amp;F66&amp;"|"&amp;G66</f>
         <v>65|387|4|0|0|</v>
       </c>
@@ -31765,7 +31765,7 @@
         <v>0</v>
       </c>
       <c r="G67" s="18"/>
-      <c r="H67" s="49" t="str">
+      <c r="H67" s="2" t="str">
         <f t="shared" si="3"/>
         <v>66|497|25|0|0|</v>
       </c>
@@ -31791,7 +31791,7 @@
         <v>0</v>
       </c>
       <c r="G68" s="18"/>
-      <c r="H68" s="49" t="str">
+      <c r="H68" s="2" t="str">
         <f t="shared" si="3"/>
         <v>67|503|15|0|0|</v>
       </c>
@@ -31817,7 +31817,7 @@
         <v>0</v>
       </c>
       <c r="G69" s="18"/>
-      <c r="H69" s="49" t="str">
+      <c r="H69" s="2" t="str">
         <f t="shared" si="3"/>
         <v>68|504|15|0|0|</v>
       </c>

</xml_diff>

<commit_message>
Fix Sec subdivision for 291
</commit_message>
<xml_diff>
--- a/src/pgsql/adif-pas/adif-pas-master.xlsx
+++ b/src/pgsql/adif-pas/adif-pas-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Git\Projects\ards-tools\src\pgsql\adif-pas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A27409E-8246-442D-8BBE-46461B459828}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FA4435-F619-4F54-99D6-ACE1FD920C8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31577,12 +31577,12 @@
         <v>1</v>
       </c>
       <c r="G60" s="20">
-        <f>O3</f>
-        <v>2</v>
+        <f>O2</f>
+        <v>1</v>
       </c>
       <c r="H60" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>59|291|21|0|1|2</v>
+        <v>59|291|21|0|1|1</v>
       </c>
       <c r="I60" s="16" t="s">
         <v>423</v>

</xml_diff>

<commit_message>
Update csv date for mat for PAS-206 (Austria)
</commit_message>
<xml_diff>
--- a/src/pgsql/adif-pas/adif-pas-master.xlsx
+++ b/src/pgsql/adif-pas/adif-pas-master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Git\Projects\ards-tools\src\pgsql\adif-pas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63936E3D-DFD7-42A9-9D60-7763248F8A5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15E0BBB-CE36-451D-8C78-E841EA860500}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12536,8 +12536,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -12832,7 +12833,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -13151,6 +13152,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -13164,33 +13171,9 @@
     <cellStyle name="Normal_pas_summary" xfId="3" xr:uid="{4AD1CB7B-29C7-477B-BDD3-7523A6CDF74E}"/>
     <cellStyle name="Note" xfId="9" builtinId="10"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -13529,8 +13512,8 @@
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36489,7 +36472,7 @@
     <col min="9" max="9" width="5.28515625" style="1" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="120" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="120" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" style="143" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="78.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="63.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="63" bestFit="1" customWidth="1"/>
@@ -36527,7 +36510,7 @@
       <c r="K1" s="119" t="s">
         <v>543</v>
       </c>
-      <c r="L1" s="119" t="s">
+      <c r="L1" s="142" t="s">
         <v>4047</v>
       </c>
       <c r="M1" s="36" t="str">
@@ -36565,7 +36548,7 @@
         <v>1240</v>
       </c>
       <c r="M2" s="50" t="str">
-        <f>G2&amp;"|"&amp;H2&amp;"|"&amp;I2&amp;"|"&amp;J2&amp;"|"&amp;IF(K2 &lt;&gt; "",TEXT(K2,"yyyy-mm-dd"),"")&amp;"|"&amp;IF(L2 &lt;&gt; "",TEXT(K2,"yyyy-mm-dd"),"")</f>
+        <f>G2&amp;"|"&amp;H2&amp;"|"&amp;I2&amp;"|"&amp;J2&amp;"|"&amp;IF(K2 &lt;&gt; "",TEXT(K2,"yyyy-mm-dd"),"")&amp;"|"&amp;IF(L2 &lt;&gt; "",TEXT(L2,"yyyy-mm-dd"),"")</f>
         <v>1|1|WC|Wien||</v>
       </c>
       <c r="O2" s="132" t="s">
@@ -36599,7 +36582,7 @@
         <v>1242</v>
       </c>
       <c r="M3" s="50" t="str">
-        <f t="shared" ref="M3:M66" si="1">G3&amp;"|"&amp;H3&amp;"|"&amp;I3&amp;"|"&amp;J3&amp;"|"&amp;IF(K3 &lt;&gt; "",TEXT(K3,"yyyy-mm-dd"),"")&amp;"|"&amp;IF(L3 &lt;&gt; "",TEXT(K3,"yyyy-mm-dd"),"")</f>
+        <f t="shared" ref="M3:M66" si="1">G3&amp;"|"&amp;H3&amp;"|"&amp;I3&amp;"|"&amp;J3&amp;"|"&amp;IF(K3 &lt;&gt; "",TEXT(K3,"yyyy-mm-dd"),"")&amp;"|"&amp;IF(L3 &lt;&gt; "",TEXT(L3,"yyyy-mm-dd"),"")</f>
         <v>2|2|HA|Hallein||</v>
       </c>
       <c r="O3" s="133" t="s">
@@ -37810,12 +37793,12 @@
       <c r="J62" s="1" t="s">
         <v>1389</v>
       </c>
-      <c r="L62" s="120">
+      <c r="L62" s="143">
         <v>41275</v>
       </c>
       <c r="M62" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>61|6|BM|Bruck/Mur||1900-01-00</v>
+        <v>61|6|BM|Bruck/Mur||2013-01-01</v>
       </c>
     </row>
     <row r="63" spans="5:13">
@@ -37914,7 +37897,7 @@
         <v>3614</v>
       </c>
       <c r="M67" s="50" t="str">
-        <f t="shared" ref="M67:M107" si="2">G67&amp;"|"&amp;H67&amp;"|"&amp;I67&amp;"|"&amp;J67&amp;"|"&amp;IF(K67 &lt;&gt; "",TEXT(K67,"yyyy-mm-dd"),"")&amp;"|"&amp;IF(L67 &lt;&gt; "",TEXT(K67,"yyyy-mm-dd"),"")</f>
+        <f t="shared" ref="M67:M107" si="2">G67&amp;"|"&amp;H67&amp;"|"&amp;I67&amp;"|"&amp;J67&amp;"|"&amp;IF(K67 &lt;&gt; "",TEXT(K67,"yyyy-mm-dd"),"")&amp;"|"&amp;IF(L67 &lt;&gt; "",TEXT(L67,"yyyy-mm-dd"),"")</f>
         <v>66|6|GB|Grobming||</v>
       </c>
     </row>
@@ -37988,12 +37971,12 @@
       <c r="J71" s="1" t="s">
         <v>4048</v>
       </c>
-      <c r="L71" s="120">
+      <c r="L71" s="143">
         <v>41275</v>
       </c>
       <c r="M71" s="50" t="str">
         <f t="shared" si="2"/>
-        <v>70|6|HF|Hartberg-Furstenfeld||1900-01-00</v>
+        <v>70|6|HF|Hartberg-Furstenfeld||2013-01-01</v>
       </c>
     </row>
     <row r="72" spans="7:13">
@@ -38123,12 +38106,12 @@
       <c r="J78" s="1" t="s">
         <v>1394</v>
       </c>
-      <c r="L78" s="120">
+      <c r="L78" s="143">
         <v>40909</v>
       </c>
       <c r="M78" s="50" t="str">
         <f t="shared" si="2"/>
-        <v>77|6|MT|Murtal||1900-01-00</v>
+        <v>77|6|MT|Murtal||2012-01-01</v>
       </c>
     </row>
     <row r="79" spans="7:13">
@@ -38205,12 +38188,12 @@
       <c r="J82" s="1" t="s">
         <v>3616</v>
       </c>
-      <c r="L82" s="120">
+      <c r="L82" s="143">
         <v>41275</v>
       </c>
       <c r="M82" s="50" t="str">
         <f t="shared" si="2"/>
-        <v>81|6|SO|Sudoststeiermark||1900-01-00</v>
+        <v>81|6|SO|Sudoststeiermark||2013-01-01</v>
       </c>
     </row>
     <row r="83" spans="5:13">
@@ -38685,6 +38668,7 @@
     <hyperlink ref="A1" location="'ENUM-LIST'!A1" display="Home" xr:uid="{EF71C3A8-0695-4D2D-BEEB-6A8603AD2B8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>